<commit_message>
Added Data Dictionary to data folder.
</commit_message>
<xml_diff>
--- a/data/data_model.xlsx
+++ b/data/data_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7becb3257e745586/3_School/BootCamp_Springboard/Data_Engineering_Path/2_open_ended_capstone/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="8_{A2C35B67-1238-490E-AAF9-6F079BE219E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B4DDF14-413C-46A1-8823-73EF66B4D20B}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="8_{A2C35B67-1238-490E-AAF9-6F079BE219E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ED16D01A-71A7-4AE8-9C72-90AF2C23DB1A}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{6FAE3B8B-F522-441F-A816-43FE04CF5C89}"/>
+    <workbookView xWindow="2543" yWindow="2543" windowWidth="18225" windowHeight="11422" activeTab="1" xr2:uid="{6FAE3B8B-F522-441F-A816-43FE04CF5C89}"/>
   </bookViews>
   <sheets>
     <sheet name="data_entities" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="42">
   <si>
     <t>dispatching_base_num</t>
   </si>
@@ -150,6 +150,18 @@
   </si>
   <si>
     <t>PowerDesigner</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -242,8 +254,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>144337</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="78" name="Ink 77">
@@ -262,7 +274,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="78" name="Ink 77">
@@ -307,8 +319,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>418238</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>565875</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>130720</xdr:rowOff>
     </xdr:to>
@@ -730,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FF4E3B-DB5C-4448-B0EF-030EF8B61EA7}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A30" sqref="A1:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
@@ -1133,14 +1145,465 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D365BA88-6155-4091-8F9B-C33F8FA19836}">
-  <dimension ref="A1"/>
+  <dimension ref="A15:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.06640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3">
+        <v>264</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3">
+        <v>264</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4">
+        <v>43831.020833333336</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4">
+        <v>43831.03125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="4">
+        <v>43831.072222222225</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="4">
+        <v>43831.043055555558</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="3">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="3">
+        <v>264</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>264</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="4">
+        <v>43817.661111111112</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="4">
+        <v>43831.019444444442</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="4">
+        <v>43817.662499999999</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="4">
+        <v>43831.022916666669</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="3">
+        <v>5</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="3">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="3">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="3">
+        <v>11.27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A43" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A44" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added data/taxi+zone_lookup and trip record user guide
</commit_message>
<xml_diff>
--- a/data/data_model.xlsx
+++ b/data/data_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7becb3257e745586/3_School/BootCamp_Springboard/Data_Engineering_Path/2_open_ended_capstone/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="184" documentId="8_{A2C35B67-1238-490E-AAF9-6F079BE219E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ED16D01A-71A7-4AE8-9C72-90AF2C23DB1A}"/>
+  <xr:revisionPtr revIDLastSave="494" documentId="8_{A2C35B67-1238-490E-AAF9-6F079BE219E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B0ED1358-4E15-4FD9-94E3-C771D89D1665}"/>
   <bookViews>
-    <workbookView xWindow="2543" yWindow="2543" windowWidth="18225" windowHeight="11422" activeTab="1" xr2:uid="{6FAE3B8B-F522-441F-A816-43FE04CF5C89}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{6FAE3B8B-F522-441F-A816-43FE04CF5C89}"/>
   </bookViews>
   <sheets>
     <sheet name="data_entities" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="49">
   <si>
     <t>dispatching_base_num</t>
   </si>
@@ -162,6 +162,27 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>LocationID</t>
+  </si>
+  <si>
+    <t>Borough</t>
+  </si>
+  <si>
+    <t>EWR</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>Newark Airport</t>
+  </si>
+  <si>
+    <t>service_zone</t>
+  </si>
+  <si>
+    <t>tax+_zone_lookup</t>
   </si>
 </sst>
 </file>
@@ -320,7 +341,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>565875</xdr:colOff>
+      <xdr:colOff>144054</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>130720</xdr:rowOff>
     </xdr:to>
@@ -358,6 +379,786 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>218214</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>61238</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>256014</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>91118</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="7" name="Ink 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3021027D-0AB4-4D6C-924A-2050135CDA55}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2514240" y="3129291"/>
+            <a:ext cx="37800" cy="29880"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="7" name="Ink 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3021027D-0AB4-4D6C-924A-2050135CDA55}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2505240" y="3120291"/>
+              <a:ext cx="55440" cy="47520"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>94014</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>71186</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>204174</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>31472</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="8" name="Ink 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97F2A519-663F-4B8C-BF74-82441EED84EC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2390040" y="2778291"/>
+            <a:ext cx="110160" cy="140760"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="8" name="Ink 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97F2A519-663F-4B8C-BF74-82441EED84EC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2381040" y="2769629"/>
+              <a:ext cx="127800" cy="158445"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>137934</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>44186</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>176814</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>162986</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="9" name="Ink 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B7505A6-4CF1-46BC-A780-A0DB68808F86}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2433960" y="2751291"/>
+            <a:ext cx="38880" cy="118800"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="9" name="Ink 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B7505A6-4CF1-46BC-A780-A0DB68808F86}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2425320" y="2742651"/>
+              <a:ext cx="56520" cy="136440"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>119801</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>119713</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>255302</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>140722</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="51" name="Ink 50">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED62D911-67D5-4001-A0C9-280547789382}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9681220" y="2304860"/>
+            <a:ext cx="782640" cy="385200"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="51" name="Ink 50">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED62D911-67D5-4001-A0C9-280547789382}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9672220" y="2295860"/>
+              <a:ext cx="800280" cy="402840"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>184241</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>18632</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>536321</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>5376</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="95" name="Ink 94">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7D03342-31F9-4EF2-9229-D05046077C95}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9745660" y="5481500"/>
+            <a:ext cx="352080" cy="168840"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="95" name="Ink 94">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7D03342-31F9-4EF2-9229-D05046077C95}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9736660" y="5472500"/>
+              <a:ext cx="369720" cy="186480"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>820641</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>75239</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>194012</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>124033</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="187" name="Ink 186">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1468D2F-3144-4BBE-BCBC-B14613AA69F4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11676340" y="1714100"/>
+            <a:ext cx="1407240" cy="595080"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="187" name="Ink 186">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1468D2F-3144-4BBE-BCBC-B14613AA69F4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11667700" y="1705460"/>
+              <a:ext cx="1424880" cy="612720"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>552388</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>178226</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>17972</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9515</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="188" name="Ink 187">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E84B64A2-C586-4C43-8E2C-A1A0AFC8E467}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="12651940" y="2909660"/>
+            <a:ext cx="255600" cy="195480"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="188" name="Ink 187">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E84B64A2-C586-4C43-8E2C-A1A0AFC8E467}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12643300" y="2901020"/>
+              <a:ext cx="273240" cy="213120"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>116894</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>60931</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>561915</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>108208</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="272" name="Ink 271">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52523801-C75E-4743-9652-D0F19972CF45}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14300740" y="2974460"/>
+            <a:ext cx="2386440" cy="2414520"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="272" name="Ink 271">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52523801-C75E-4743-9652-D0F19972CF45}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14292100" y="2965820"/>
+              <a:ext cx="2404080" cy="2432160"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>411181</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1439</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>543413</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>45939</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="275" name="Ink 274">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D6847C4-FDC3-4FFC-9614-AC904F742114}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="10619740" y="1640300"/>
+            <a:ext cx="5401800" cy="1683360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="275" name="Ink 274">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D6847C4-FDC3-4FFC-9614-AC904F742114}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10610740" y="1631300"/>
+              <a:ext cx="5419440" cy="1701000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>311400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>3304</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228855</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>12050</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="282" name="Ink 281">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F870A4C-AA11-4EA6-993C-40895ED8FAAF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8578540" y="1824260"/>
+            <a:ext cx="5834160" cy="4379040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="282" name="Ink 281">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F870A4C-AA11-4EA6-993C-40895ED8FAAF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8569541" y="1815260"/>
+              <a:ext cx="5851799" cy="4396680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>204594</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>111664</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>226695</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>42495</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="283" name="Ink 282">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DFB7332-02CA-44BD-B16A-1C1710067F06}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13741300" y="1932620"/>
+            <a:ext cx="669240" cy="2844360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="283" name="Ink 282">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DFB7332-02CA-44BD-B16A-1C1710067F06}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13732660" y="1923980"/>
+              <a:ext cx="686880" cy="2862000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>696441</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>165857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>413235</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>55056</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="295" name="Ink 294">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CF2C9EB-1AA1-44AA-B406-ECCD50EA21D1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11552140" y="2533100"/>
+            <a:ext cx="4986360" cy="3166920"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="295" name="Ink 294">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CF2C9EB-1AA1-44AA-B406-ECCD50EA21D1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11543499" y="2524460"/>
+              <a:ext cx="5004001" cy="3184560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -440,6 +1241,541 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">152 269 2904 0 0,'0'0'128'0'0,"5"-4"-128"0"0,3 0 0 0 0,-2 1 440 0 0,2-5 56 0 0,-3 4 16 0 0,3 0 0 0 0,-4 0-416 0 0,6-4-96 0 0,-6 4 0 0 0,5 0 0 0 0,-5 0 0 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink10.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-12-08T23:12:46.880"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">14291 4675 8896 0 0,'0'0'433'0'0,"10"-5"62"0"0,22-23-157 0 0,0 10 429 0 0,33-15 0 0 0,-35 19-775 0 0,0-1 0 0 0,-2-2 0 0 0,0 0 0 0 0,0-2 0 0 0,-2-1 0 0 0,0-1 0 0 0,43-48 0 0 0,-16 10 668 0 0,65-97 0 0 0,-98 126-419 0 0,-1-2 0 0 0,-2 0 1 0 0,-2 0-1 0 0,-1-2 0 0 0,16-55 1 0 0,-23 62-107 0 0,-1 0 1 0 0,-2 0-1 0 0,-1-1 1 0 0,-1 0-1 0 0,-1 0 1 0 0,-1 1-1 0 0,-2-1 1 0 0,0 0 0 0 0,-2 1-1 0 0,-2-1 1 0 0,-15-49-1 0 0,9 48-164 0 0,0 2-1 0 0,-2 0 1 0 0,0 0-1 0 0,-31-40 1 0 0,4 16-111 0 0,-50-50 1 0 0,42 55 244 0 0,-88-63 1 0 0,31 28-228 0 0,36 28 260 0 0,-3 3 0 0 0,-117-60 1 0 0,-43 1 277 0 0,-6 16-221 0 0,38 15-137 0 0,67 27-47 0 0,-65-28-12 0 0,-28-16-27 0 0,-116-51 72 0 0,65 10-44 0 0,-66-22 0 0 0,173 80 0 0 0,-197-82 0 0 0,-95-8-240 0 0,34 25 193 0 0,-7 20 31 0 0,229 70 15 0 0,-203-46 1 0 0,140 42 59 0 0,-82-16-30 0 0,-702-117-29 0 0,813 150 6 0 0,-468-86-98 0 0,70-2-168 0 0,-894-86-259 0 0,687 118-609 0 0,488 52 1185 0 0,-537 4 0 0 0,367 79 7 0 0,24 52-480 0 0,492-88 412 0 0,-480 124-256 0 0,120 14 553 0 0,317-115 13 0 0,-50 33 0 0 0,82-45-577 0 0,2 1 0 0 0,0 1 0 0 0,1 2 0 0 0,-32 34 0 0 0,18-17-1601 0 0,25-25 994 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="876.79">373 333 12640 0 0,'-2'-1'107'0'0,"-1"0"1"0"0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-3-4-1 0 0,-12-10 105 0 0,15 16-238 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,2 1 1 0 0,0 19-650 0 0,2 0 0 0 0,0 1 1 0 0,13 39-1 0 0,-10-40 542 0 0,35 114-16 0 0,-22-74 110 0 0,-7-28 333 0 0,1 0 1 0 0,1-1 0 0 0,2-1-1 0 0,1 0 1 0 0,34 45 0 0 0,-49-73-191 0 0,-1-1-4 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,2 4 375 0 0,-3-7-455 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,1 1 0 0 0,-3-2 0 0 0,-3-4-23 0 0,-10-8-388 0 0,0-1 0 0 0,1-1-1 0 0,1 0 1 0 0,1-1 0 0 0,0-1 0 0 0,-15-30 0 0 0,-3-15-199 0 0,3-1-1 0 0,-37-126 1 0 0,60 165 701 0 0,1 0-1 0 0,1 0 0 0 0,0-45 1 0 0,1 56 222 0 0,1 28 0 0 0,4 17-232 0 0,-1 1 1 0 0,-1-1 0 0 0,-2 0-1 0 0,-2 1 1 0 0,-5 30 0 0 0,-2-12 137 0 0,-3-1 1 0 0,-23 61 0 0 0,-26 26 925 0 0,29-67-594 0 0,-6 10-112 0 0,22-47-452 0 0,1 1 0 0 0,2 1 0 0 0,-13 41 0 0 0,27-73-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1 0 0 0,0 2 0 0 0,1-2-6 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,3 0 0 0 0,6 0-14 0 0,-1-1 0 0 0,0 1 0 0 0,1-2 0 0 0,16-1 0 0 0,-24 1 18 0 0,139-23-450 0 0,-93 13-509 0 0,1 3-1 0 0,52-2 1 0 0,-70 10-3042 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink11.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-12-08T23:03:08.555"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1453 8811 12392 0 0,'0'0'364'0'0,"-1"0"-8"0"0,-3 1-227 0 0,1 0-137 0 0,3 0-10 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0 1 4 0 0,53 300-237 0 0,-51-281 238 0 0,19 270 13 0 0,-19-87 538 0 0,-8-1 1 0 0,-56 351 0 0 0,35-414-23 0 0,-24 168-82 0 0,47-274-4106 0 0,0-2-1286 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1137.14">1474 8577 11312 0 0,'-31'-1'384'0'0,"22"0"-213"0"0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-17 3 1 0 0,25-3-172 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,4 3 0 0 0,-6-3 0 0 0,5 2-20 0 0,0-1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,4 0 0 0 0,8 0-47 0 0,12 0-8 0 0,-1-2 1 0 0,53-9-1 0 0,-42 5 67 0 0,349-66-79 0 0,-95 17-85 0 0,679-93 11 0 0,-623 108 249 0 0,-31 6-44 0 0,376-24 20 0 0,-446 57-128 0 0,-198 4 77 0 0,1 3 0 0 0,93 21 1 0 0,-125-21 1 0 0,1 0 0 0 0,-1 0 1 0 0,0 2-1 0 0,-1 0 0 0 0,0 1 0 0 0,0 0 1 0 0,-1 2-1 0 0,0 0 0 0 0,-1 1 1 0 0,0 1-1 0 0,-1 0 0 0 0,0 1 1 0 0,-1 0-1 0 0,-1 1 0 0 0,0 1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-2 1 1 0 0,14 37-1 0 0,-10-13 144 0 0,-3 0-1 0 0,-1 0 1 0 0,-2 0 0 0 0,0 56-1 0 0,-18 170 873 0 0,-36 86-150 0 0,5-59 317 0 0,-26 389-596 0 0,48-198-298 0 0,35 0-291 0 0,28-137-13 0 0,-39-329 0 0 0,-2-14 12 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,-2 10 0 0 0,3-13 17 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,-3-1 0 0 0,-22 0 227 0 0,0-1 0 0 0,-1-2-1 0 0,1 0 1 0 0,-50-15-1 0 0,16 4 75 0 0,-26-5 45 0 0,-59-10-52 0 0,20 6-505 0 0,-84-13 120 0 0,-12 0 62 0 0,146 26 2 0 0,-349-34 590 0 0,244 41 72 0 0,-198 24 0 0 0,340-17-578 0 0,-205 25 116 0 0,148-14-149 0 0,-293 57 36 0 0,270-45-477 0 0,-132 52 1 0 0,210-64 348 0 0,-31 12-69 0 0,-86 44 0 0 0,-31 29 65 0 0,127-71-14 0 0,-74 22 0 0 0,108-42-42 0 0,-51 9 0 0 0,68-16 95 0 0,1-1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-15-4 0 0 0,20 4 1 0 0,0 0-1 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-2-7 1 0 0,0-5-47 0 0,0 0 0 0 0,1 0 1 0 0,1-27-1 0 0,5-51-167 0 0,26-153-1 0 0,50-153-1289 0 0,-34 184 277 0 0,30-128-2606 0 0,-46 224 2392 0 0,-7 17-10 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2365.05">2040 8726 9128 0 0,'-5'-2'239'0'0,"4"2"-127"0"0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,-2-3 482 0 0,3 5-596 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 2 0 0 0,0 2-29 0 0,-2 3 16 0 0,1 0 0 0 0,0 0 0 0 0,-1 15 0 0 0,-1 3-1 0 0,-1 3 16 0 0,-3 38 0 0 0,7-54 0 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,1 0 0 0 0,5 20 0 0 0,-7-32 12 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,2 0 1 0 0,-2 1 27 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,3 2 0 0 0,-4-1-14 0 0,1-1-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,3 1-1 0 0,13 0 38 0 0,0-1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-2 0 0 0,28-6 0 0 0,-25 5-61 0 0,-16 3-52 0 0,1 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,4-3 0 0 0,20-12-648 0 0,-16 11 340 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2751.01">2520 8915 12528 0 0,'-16'-7'1249'0'0,"8"9"-1526"0"0,8-2 198 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 1 39 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,2 1 1 0 0,26 14 214 0 0,-18-11-397 0 0,-10-4 289 0 0,1 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,3-2 1 0 0,-4 2-23 0 0,1 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-22 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,1-1 54 0 0,7-13-26 0 0,-9 14-68 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,-2-2-106 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,-7-5 0 0 0,0 0 16 0 0,6 5 61 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,-10-1 0 0 0,-5-1-2910 0 0,12 2-219 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3276.08">2998 8804 9184 0 0,'-3'-3'196'0'0,"-17"-14"505"0"0,19 17-686 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-2 1 0 0 0,1 0-14 0 0,-2 2-1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-3 5 0 0 0,1 1-25 0 0,0 1-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,0 1 1 0 0,1-2 0 0 0,1 2-1 0 0,-1 0 1 0 0,2-1 0 0 0,0 1 0 0 0,0 0-1 0 0,3 16 1 0 0,-2-27 203 0 0,1 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,5 1-1 0 0,-1 2 93 0 0,-2-3-230 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,3-2 1 0 0,-3 2 36 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0-4 0 0 0,0 2-125 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,2-9 0 0 0,5-27 1913 0 0,1 50-1762 0 0,14 19-572 0 0,-22-27 201 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,1 2 0 0 0,4 4-945 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3801.1">3300 8717 7080 0 0,'0'0'530'0'0,"-5"-4"-324"0"0,1 3-78 0 0,0-1 1 0 0,0 1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-5 3 1 0 0,4 0-127 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 8 1 0 0,2-5 15 0 0,0 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,4 15 1 0 0,-4-20-2 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,1-1 0 0 0,5 4 1 0 0,-8-6 42 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,2-2-1 0 0,5-2 196 0 0,-1-1 0 0 0,0-1 0 0 0,7-7 1 0 0,-3 4-93 0 0,-4 1-333 0 0,1 0 0 0 0,8-11 0 0 0,-4 4-1745 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4437.39">3509 8797 9880 0 0,'-14'0'489'0'0,"5"-1"-542"0"0,-1 1 1 0 0,1 0-1 0 0,-1 1 1 0 0,-9 2-1 0 0,16-1 43 0 0,1 0-4 0 0,0-1-26 0 0,1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0 2 0 0 0,-1-3 179 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,0 1 6 0 0,1-3-127 0 0,0 2-16 0 0,-4-1 6 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,0 1 94 0 0,15-10 460 0 0,-14 9-548 0 0,0 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,3-1 0 0 0,-2 1 156 0 0,-1 0-115 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,2 1 0 0 0,47 61-91 0 0,-49-62-85 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,3 1 0 0 0,-2-1-620 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4772.66">3718 8579 15344 0 0,'0'0'348'0'0,"-12"9"991"0"0,11-8-1336 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,1 2 0 0 0,9 28 127 0 0,-5-17-119 0 0,7 20-249 0 0,2-1 0 0 0,22 40 0 0 0,4 10-2929 0 0,-31-61 1985 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4773.66">3674 8728 15752 0 0,'0'0'1573'0'0,"18"1"-1419"0"0,21 10-395 0 0,56 18-512 0 0,-88-27 285 0 0,0 1 1 0 0,-1-2-1 0 0,13 3 0 0 0,0-2-4842 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5127.28">4037 8710 15576 0 0,'0'0'761'0'0,"-8"11"189"0"0,8-7-988 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 0-1 0 0,2 4 1 0 0,-2-5 11 0 0,12 26-768 0 0,1 0-1 0 0,34 46 1 0 0,-44-70 772 0 0,-4-3 15 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,3 2 1 0 0,0-3 92 0 0,-4 1-37 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1-7 67 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,-1 0 1 0 0,-2-9 0 0 0,2 10-196 0 0,1 1 0 0 0,-2 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,0 0 0 0 0,-7-9 0 0 0,9 13 50 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,-3 1-1 0 0,-7 1 18 0 0,11-2 45 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-5 4 1 0 0,7-5-33 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 1 0 0 0,16 7-1812 0 0,15-6-1798 0 0,-15-3 1743 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5882.76">4396 8707 12672 0 0,'0'0'289'0'0,"-3"0"694"0"0,-2 0-882 0 0,1 0-68 0 0,3 0 622 0 0,0 0-655 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 2 0 0 0,0 0 7 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 2-1 0 0,1 4 20 0 0,0 1-1 0 0,0 0 0 0 0,3 11 1 0 0,-3-16-36 0 0,3 21 31 0 0,2-1 0 0 0,9 32 1 0 0,-14-56-35 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,4-9-199 0 0,0-14 370 0 0,-3 22-166 0 0,2-24-13 0 0,5-17-145 0 0,-7 27 508 0 0,-1 11 810 0 0,1 11-1222 0 0,-1-7 57 0 0,1 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,14-5 226 0 0,14-10 543 0 0,-28 15-747 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,3 4-19 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,2 8-1 0 0,-2-6-28 0 0,2 4 51 0 0,-2 0 1 0 0,3 15 0 0 0,-4-17-124 0 0,0 0 1 0 0,1-2-1 0 0,0 1 0 0 0,7 16 1 0 0,-7-20-572 0 0,-3-4 208 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,2 2-1 0 0,2 0-1383 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6246.79">4669 8809 10336 0 0,'0'0'2218'0'0,"3"14"-892"0"0,-1 53-1182 0 0,-2-62-95 0 0,0 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,3 7 0 0 0,-4-12 271 0 0,7-7 928 0 0,-5 1-1195 0 0,1 0 0 0 0,-1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,0-2 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-5-13-1 0 0,4 16-16 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-4-2-1 0 0,5 3 165 0 0,0 1-33 0 0,1 0-184 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 2-1 0 0,1 19-220 0 0,0-14 251 0 0,0 0 0 0 0,1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,6 7 0 0 0,-7-12-276 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,4 0 0 0 0,3 0-4845 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6968.15">1448 9426 13944 0 0,'0'-1'48'0'0,"1"0"0"0"0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,2 0-1 0 0,27-10-238 0 0,-25 9 254 0 0,30-9-388 0 0,0 3 1 0 0,45-7-1 0 0,-45 10 134 0 0,125-11-512 0 0,-87 11 653 0 0,61-2 225 0 0,27-3-144 0 0,122 0-337 0 0,-112 8 405 0 0,394-45 247 0 0,-4-33 1295 0 0,-211 40-484 0 0,-263 32-1093 0 0,287 2 224 0 0,-209 8-981 0 0,13-2-1857 0 0,-91 0-2355 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11013.85">2061 9881 11376 0 0,'-4'3'123'0'0,"1"-1"1"0"0,0 1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-3 7 1 0 0,1 2-136 0 0,-5 23 1 0 0,0 1 24 0 0,-6 28-140 0 0,14-61 79 0 0,1-3-140 0 0,-11-21-1026 0 0,3 3 1334 0 0,0-3 0 0 0,1 1 0 0 0,1-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1-32 0 0 0,5 30 15 0 0,0-1 0 0 0,6-41 1 0 0,-3 51 37 0 0,0 1 1 0 0,2-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,1 0-1 0 0,9-16 1 0 0,-13 27-156 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,2-2 1 0 0,-4 3-19 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,2 4 47 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-3 11 1 0 0,2-9-330 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,2 7 0 0 0,0-3-768 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11430.76">2276 9558 17567 0 0,'-2'-1'183'0'0,"1"0"-119"0"0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-2 1 0 0 0,1 0-123 0 0,5 9-785 0 0,15 40-992 0 0,-6-16-166 0 0,13 52 1 0 0,-21-68 1312 0 0,-2-11 261 0 0,0 1 0 0 0,-1-1 0 0 0,1 13 0 0 0,-4-18 394 0 0,-3-5 27 0 0,-1-4 26 0 0,5 6 374 0 0,12-10 891 0 0,-8 11-1263 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,2 3 1 0 0,29 32 74 0 0,-32-35-89 0 0,17 18-473 0 0,26 22 0 0 0,-37-37-3623 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11799.77">2310 9736 14024 0 0,'-2'-2'304'0'0,"-1"2"448"0"0,-2-4-272 0 0,7-1-480 0 0,1-1-128 0 0,2-1-48 0 0,0 0-8 0 0,6 0 0 0 0,-3-2-216 0 0,5-1-48 0 0,0-2 0 0 0,2 1-5040 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12479.69">2935 9419 9504 0 0,'-3'-3'123'0'0,"1"1"0"0"0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2-3 0 0 0,4 5-54 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,-2-2-1 0 0,3 2 447 0 0,1-1-389 0 0,0-2-87 0 0,0 1-1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-2-5-1 0 0,2 6-92 0 0,1 120-444 0 0,3 200 852 0 0,15 188-161 0 0,-29-52 201 0 0,-1 13 566 0 0,18-353-1467 0 0,25 133 1 0 0,-26-223 36 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15137.41">3242 9540 12528 0 0,'-3'0'1356'0'0,"-1"-2"-1376"0"0,3 2-148 0 0,4 14-555 0 0,9 40 328 0 0,-4-21 370 0 0,-2-1 1 0 0,-1 1-1 0 0,1 33 1 0 0,-6-65 321 0 0,-1-17-666 0 0,-4-154-2617 0 0,5 126 2264 0 0,0 35 673 0 0,0 0 1 0 0,1 0 0 0 0,0 0 0 0 0,5-17-1 0 0,-6 25 94 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,1 1-23 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,2 3 1 0 0,20 24 143 0 0,-18-22-112 0 0,0 0 1 0 0,8 11-1 0 0,-10-12-17 0 0,3 5 71 0 0,1 1 1 0 0,15 16 0 0 0,-21-25 13 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,2 1 1 0 0,-4-1-54 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0-1 0 0 0,1-1 10 0 0,-1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-6 0 0 0,-4-15-401 0 0,0-1 0 0 0,-2 1 1 0 0,-11-33-1 0 0,14 48-59 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,3-12 0 0 0,-1 11-449 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15587.33">3734 9496 13216 0 0,'-8'3'1326'0'0,"7"-2"-1337"0"0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 3 0 0 0,-1 7 9 0 0,-3 24-214 0 0,3-24 79 0 0,0 0-1 0 0,-2 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,-6 19-1 0 0,8-29 49 0 0,-1-10-313 0 0,-7-30-68 0 0,1-1-1 0 0,-4-75 0 0 0,12 76 3061 0 0,0 38-2571 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,7 3 163 0 0,-2-1-75 0 0,-3-1-110 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,3 5 1 0 0,1 3 15 0 0,0 0 0 0 0,6 10 0 0 0,1 8-20 0 0,-2-1-1 0 0,14 46 1 0 0,-4-10 40 0 0,-17-52-11 0 0,-3-5-518 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,4 6 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15926.42">3676 9451 14112 0 0,'3'1'1529'0'0,"37"36"-1962"0"0,-11-16 46 0 0,26 19-2756 0 0,-37-30 1961 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16402.07">3897 9590 13448 0 0,'-13'10'1458'0'0,"12"-8"-1416"0"0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 2 1 0 0,11 35 309 0 0,-8-28-453 0 0,-2-3 107 0 0,0-2-73 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,8 10 0 0 0,-11-15 63 0 0,0 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1-1-13 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,5-33-400 0 0,-5 33 410 0 0,1-73 600 0 0,-1 43 1503 0 0,1 34-2036 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 3 1 0 0,0-4-40 0 0,1 9-88 0 0,11 30 37 0 0,-12-37 24 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,3 3-1 0 0,-4-4-45 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,10-18-484 0 0,6-13 2817 0 0,-15 32-2277 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 1-1 0 0,0-1 11 0 0,0 1-1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,1 0 0 0 0,10-3-60 0 0,-6 1-306 0 0,0 1 0 0 0,0 0 0 0 0,9-1 0 0 0,-16 2 318 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-6-7-461 0 0,-14-8 1407 0 0,20 15-895 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,4 8 51 0 0,-2-6-65 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 1 0 0,1 1-1 0 0,3 1 1 0 0,29 10-5 0 0,-16-8 5 0 0,-12-2-79 0 0,0-2 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0-2-1 0 0,0 1 1 0 0,10-6-1 0 0,-3-3-5260 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29302.65">3345 10964 7168 0 0,'0'0'728'0'0,"0"-9"-307"0"0,0 8-421 0 0,0 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,8 6 10 0 0,-5 1 11 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,3 13 0 0 0,8 46 99 0 0,-14-63-119 0 0,0 10 9 0 0,-1-14 108 0 0,-16-12-77 0 0,11 4-289 0 0,1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,2-1 0 0 0,-6-13 0 0 0,5 6-165 0 0,-1 2 0 0 0,2-2-1 0 0,0 0 1 0 0,-1-24 0 0 0,3 29 654 0 0,1 0-1 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,0 1 0 0 0,1 0 1 0 0,4-12-1 0 0,-6 19-152 0 0,0-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-2 1 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,4-1 1 0 0,-2 1-42 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,4 2-1 0 0,1 0-16 0 0,-1 0 0 0 0,1 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,7 7 0 0 0,-12-9-13 0 0,0-1 0 0 0,0 2 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-3 5 0 0 0,-1 0 275 0 0,0 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,-13 13 0 0 0,-5 7-198 0 0,-10 9 32 0 0,16-18-3500 0 0,9-7-309 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29996.06">3823 10871 9728 0 0,'0'0'474'0'0,"0"0"-204"0"0,-1-1-197 0 0,1 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,-3 3-195 0 0,1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-5 8-1 0 0,6-7 181 0 0,-3 3-77 0 0,0 0 0 0 0,1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,-4 16 0 0 0,6-20 49 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,4 9 0 0 0,-7-14-13 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,3 0 0 0 0,-2 0 48 0 0,1 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,3-1-1 0 0,0-2 87 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,4-5 1 0 0,-4 3-112 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-3-8 0 0 0,2 10-64 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0 1 1 0 0,0-1-1 0 0,-6 0 1 0 0,10 0-72 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0 9-1073 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="31028.72">4063 10772 10680 0 0,'0'0'1072'0'0,"5"14"-968"0"0,-5 0-460 0 0,1-10 163 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 6 1 0 0,-11 66-501 0 0,5-20 511 0 0,5-39 331 0 0,1 0 0 0 0,0 0-1 0 0,3 28 1 0 0,-1-41-62 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 0 0 0 0,3 5-1 0 0,-4-7-36 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,12-1 164 0 0,0 0-1 0 0,0-2 1 0 0,-1 1-1 0 0,1-2 0 0 0,17-6 1 0 0,5-1 290 0 0,40-17-171 0 0,-59 20-575 0 0,1 1 0 0 0,-1 2 0 0 0,1 0 0 0 0,0 0 0 0 0,20-1 0 0 0,-10 4-609 0 0,-5 6-10 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-53624.61">2163 967 5608 0 0,'2'12'129'0'0,"-1"0"1"0"0,0 13-1 0 0,-1-13-165 0 0,1 0 0 0 0,2 12 0 0 0,-1-6 0 0 0,0 1 0 0 0,-1 26 0 0 0,-1-34 74 0 0,-3 6 134 0 0,-7-47 1063 0 0,4 4-385 0 0,3 13-542 0 0,1 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,0 1 1 0 0,1-16-1 0 0,0 18-241 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,8-16 0 0 0,-7 17-110 0 0,0 1 0 0 0,1-1 0 0 0,0 2 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,13-7 0 0 0,-18 12 13 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,2 5 1 0 0,4 8 141 0 0,-2 1 0 0 0,1-2 0 0 0,-2 2 0 0 0,0 1 0 0 0,3 19 0 0 0,-3-1 255 0 0,-1 45 0 0 0,-3-70-192 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,-5 13-1 0 0,6-18-82 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-6 0 1 0 0,-2-2-227 0 0,6-1-3572 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-53252.77">2635 1123 13344 0 0,'0'0'390'0'0,"3"-16"156"0"0,-1 13-658 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,5-3-1 0 0,3-7 19 0 0,-8 11 139 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,4-2 0 0 0,-6 3-87 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-3 14-37 0 0,-14 81-2250 0 0,17-87-1562 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-52876.65">2812 1204 13160 0 0,'0'0'297'0'0,"10"14"846"0"0,5-7-1165 0 0,0-3-1 0 0,0 1 1 0 0,18 4 0 0 0,-28-8-97 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,9-4-1 0 0,-14 6 98 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-2 0 0 0,0 0 27 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,-2-4 1 0 0,-1-2 193 0 0,-1 1 0 0 0,-11-12 0 0 0,16 17-197 0 0,-63-55 1170 0 0,56 50-1105 0 0,5 5-61 0 0,0 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-3 0 0 0,-7-13-17 0 0,8 18-32 0 0,0-3-6 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,4-2 1 0 0,-2 1-131 0 0,1 1-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,5-2 0 0 0,8-7-682 0 0,22-13-2663 0 0,-31 18 2630 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-52380.66">3177 1062 11256 0 0,'0'0'857'0'0,"5"9"-474"0"0,-2-4-483 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 8 1 0 0,1 52 401 0 0,-2-31-30 0 0,0 18-501 0 0,-1-47 218 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-5 9 0 0 0,5-14-8 0 0,1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-2-1 0 0,-2-1 13 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-3-5 1 0 0,-2-6-64 0 0,1 0 1 0 0,1-1 0 0 0,0 1-1 0 0,-2-17 1 0 0,-6-66-311 0 0,11 78 389 0 0,-3-19-65 0 0,2-80 0 0 0,4 104 170 0 0,0 1 0 0 0,1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,9-14 0 0 0,-12 23-77 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,6-3-1 0 0,-9 3-22 0 0,1 2-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,3 3 1 0 0,-4-2-12 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,0 3 0 0 0,0 3 9 0 0,-1 0 0 0 0,0 0 0 0 0,-2 9 0 0 0,1-9 76 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,0 0-1 0 0,-7 8 0 0 0,-3 1 218 0 0,0-2 0 0 0,-31 22 0 0 0,28-26-2255 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-51820.21">3366 798 10800 0 0,'2'10'812'0'0,"7"17"-1065"0"0,-1 1 0 0 0,-2 0 0 0 0,-1-1 1 0 0,-2 2-1 0 0,-1 0 0 0 0,-2 53 0 0 0,-2-63-525 0 0,-6 28-1 0 0,5-40 2202 0 0,3-15-191 0 0,2-17-203 0 0,27-164-414 0 0,-26 174-605 0 0,-3 8 15 0 0,1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,6-11 1 0 0,-8 16 21 0 0,-1 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,1 0 0 0 0,-1 0-25 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,2 1 1 0 0,2 4-49 0 0,0 1 0 0 0,0-1 0 0 0,3 11 0 0 0,-6-16 56 0 0,57 179-642 0 0,-44-131 304 0 0,8-8-876 0 0,-31-51-2893 0 0,-12-12 2722 0 0,-22-12 1450 0 0,34 28 814 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1 0-1 0 0,-12-4 1 0 0,79 18 266 0 0,4 0-1378 0 0,-39-6-490 0 0,-1 0 0 0 0,0 1 0 0 0,28 8 0 0 0,-45-10 157 0 0,1-1-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,6 1-1 0 0,-9-3-121 0 0,2-6 1 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-51479.89">3910 746 7968 0 0,'0'0'233'0'0,"9"15"1846"0"0,-5-10-1978 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 7 0 0 0,0 13-101 0 0,-5 51 0 0 0,2-65 107 0 0,2-6-176 0 0,-1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-5 10 0 0 0,5-12-197 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-51140.72">3624 877 11600 0 0,'9'-3'881'0'0,"61"-14"-490"0"0,-31 5-403 0 0,32-7-134 0 0,-1-3 0 0 0,76-36 0 0 0,-103 37-2788 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-50783.52">4462 772 17167 0 0,'-11'-11'742'0'0,"9"10"-691"0"0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-2-1 0 0,1 2-62 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1 0 0 0,-3-1 0 0 0,1 1-251 0 0,0 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-5 4-1 0 0,-3 5-446 0 0,0 1 1 0 0,-11 16-1 0 0,9-11 107 0 0,1-2 156 0 0,-38 53-26 0 0,41-56 775 0 0,1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-4 13 0 0 0,10-24-248 0 0,-1 0-1 0 0,0-1 1 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,1 3 0 0 0,0-2-32 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,5 0-1 0 0,-1 1-53 0 0,1-1 0 0 0,0-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,12-5 1 0 0,23-15-321 0 0,-15 3-3078 0 0,-6 2-495 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-50446.97">4549 482 12872 0 0,'-1'0'49'0'0,"1"0"0"0"0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,-1 7 271 0 0,6 21-765 0 0,-2-17 441 0 0,-1 21-296 0 0,-1-1 0 0 0,-5 42 0 0 0,0-1 510 0 0,0 134-337 0 0,5-206 141 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,8-10 229 0 0,6-18-214 0 0,39-94 77 0 0,-50 117-17 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,4-4-1 0 0,-7 9-75 0 0,1-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 2-1 0 0,4 5 70 0 0,-1 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,1-1 0 0 0,3 17-1 0 0,8 44-154 0 0,-7-30 103 0 0,-3-10-244 0 0,7 26-131 0 0,-11-49-67 0 0,1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,5 6-1 0 0,-1-5-4134 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-49829.09">1214 1969 15136 0 0,'0'-2'881'0'0,"0"1"-877"0"0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1-9 0 0,13-7-234 0 0,-1 1 1 0 0,1 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,26-4 0 0 0,-3 0 108 0 0,319-49-2183 0 0,5 29 1976 0 0,-114 17 508 0 0,267-25 245 0 0,-13-67 97 0 0,-13-47 436 0 0,53 1-901 0 0,15 52-103 0 0,-510 91-36 0 0,533-52-1095 0 0,-509 55-1960 0 0,-1-1-979 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-62696.16">6001 2391 10736 0 0,'-6'-3'632'0'0,"7"7"-242"0"0,2 5-503 0 0,8 49 64 0 0,6 94-1 0 0,-11 61-508 0 0,-5-142 330 0 0,-13 618 79 0 0,2-384 114 0 0,10 383 70 0 0,3-173 10 0 0,-100 805 4967 0 0,58-978-6010 0 0,36-317-4280 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-60899.74">6118 2327 11112 0 0,'5'-1'117'0'0,"-1"1"1"0"0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,4-3 1 0 0,15-3 167 0 0,263-69-85 0 0,-171 48-145 0 0,168-37-219 0 0,-162 39 171 0 0,310-58-254 0 0,533-138-9 0 0,-670 148 68 0 0,522-59 0 0 0,-223 88 204 0 0,61 62 203 0 0,-209 1-110 0 0,412 5-61 0 0,-62 37-400 0 0,-764-56 354 0 0,-1 1 0 0 0,0 2 0 0 0,33 12 0 0 0,-47-14 52 0 0,-1 1 0 0 0,0 2-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 1 0 0 0,-1 1 0 0 0,18 16-1 0 0,-20-15-3 0 0,0 1 0 0 0,-1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,0 2 0 0 0,-1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,4 31 0 0 0,-4-10-42 0 0,-2-1 0 0 0,-2 1 1 0 0,-2 0-1 0 0,-7 55 0 0 0,-78 532 222 0 0,57-423-194 0 0,6-45-36 0 0,-59 430 0 0 0,-54 576 80 0 0,98-514 88 0 0,70 89 24 0 0,-29-704-12 0 0,1-1 1 0 0,2 0 0 0 0,0-2 0 0 0,17 46 0 0 0,-16-58-181 0 0,-5-13 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 8 0 0 0,-4-12-3 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 1 0 0,-2 1 3 0 0,-1 0 1 0 0,0-1-1 0 0,-11 0 1 0 0,-190-26 1052 0 0,-77-4 204 0 0,-156 47-675 0 0,-9 30-589 0 0,-10 2 92 0 0,-622 7 3188 0 0,-11-47-1646 0 0,695-9-1912 0 0,-643 3-830 0 0,850 3 1182 0 0,-239 37 0 0 0,198 9-303 0 0,5 18-851 0 0,34 4-123 0 0,74-15 1064 0 0,71-33 4 0 0,-65 24 0 0 0,103-47 193 0 0,1 0 0 0 0,-1-1 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,0-2 0 0 0,-13 1 1 0 0,18-2-28 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,1-1 0 0 0,-6-5-1 0 0,1 0-86 0 0,1-1-1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-2-14 0 0 0,1 3-77 0 0,2 0 0 0 0,0-1-1 0 0,2 0 1 0 0,4-39 0 0 0,33-144 129 0 0,17 0-34 0 0,-14 59 10 0 0,3-28-124 0 0,-16 58-4522 0 0,-11 45-588 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-58484.11">1584 450 9672 0 0,'0'1'82'0'0,"1"1"0"0"0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,2 4 0 0 0,2 6 188 0 0,10 32-309 0 0,-2 1 0 0 0,-3-1 0 0 0,10 84 0 0 0,1 262 176 0 0,-26 1 738 0 0,-29 140 524 0 0,-53-5 546 0 0,-20-90-1341 0 0,99-400-1696 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-57337.18">1755 531 5608 0 0,'1'2'27'0'0,"0"0"0"0"0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,2 1 0 0 0,26 10-53 0 0,-28-12 46 0 0,18 6 149 0 0,-1-1 0 0 0,1-2 1 0 0,29 4-1 0 0,65-1 1081 0 0,-93-6-1001 0 0,57 0 541 0 0,79-11 0 0 0,78-20-357 0 0,480-133-275 0 0,-314 46-136 0 0,-20 6 16 0 0,2 16-18 0 0,-282 76 18 0 0,0 4 0 0 0,2 4 0 0 0,200 4 0 0 0,-272 10-206 0 0,0 1 0 0 0,0 2 0 0 0,-1 0 1 0 0,0 2-1 0 0,55 21 0 0 0,-70-22 80 0 0,0 1-1 0 0,0 0 1 0 0,-1 1-1 0 0,0 0 0 0 0,-1 2 1 0 0,1 0-1 0 0,-2 0 1 0 0,1 1-1 0 0,-2 1 1 0 0,0 0-1 0 0,0 0 1 0 0,15 25-1 0 0,-15-18 0 0 0,-1 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,0 1-1 0 0,-2 0 1 0 0,4 23 0 0 0,-5-15 109 0 0,-1 1 0 0 0,-2 0 0 0 0,-3 52 1 0 0,-3-27 272 0 0,-15 65 0 0 0,-21 50 602 0 0,38-161-843 0 0,-156 574 1566 0 0,26-114-377 0 0,117-417-1196 0 0,-82 405 469 0 0,34 4-444 0 0,17 250 150 0 0,46-693-183 0 0,3 122 227 0 0,-1-111 92 0 0,1-1 1 0 0,14 52-1 0 0,-16-75-305 0 0,1 1 102 0 0,-1 0 0 0 0,2 0 1 0 0,-1-1-1 0 0,5 9 1 0 0,-21-36 2504 0 0,7 11-2467 0 0,-1 0-1 0 0,-17-17 1 0 0,8 12-153 0 0,-1 2 0 0 0,0 0 0 0 0,-1 3 1 0 0,-22-13-1 0 0,5 6-140 0 0,-57-20 0 0 0,47 24-10 0 0,1 2 0 0 0,-1 2 1 0 0,-92-8-1 0 0,-144 12 85 0 0,-425 51 308 0 0,284-11 28 0 0,-380 47-859 0 0,728-71 483 0 0,-102 19 237 0 0,95-15-99 0 0,54-10-75 0 0,-1 1 0 0 0,-43 14 0 0 0,20-3 100 0 0,-107 18 0 0 0,100-23 118 0 0,51-10-170 0 0,-1 0-1 0 0,1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-12-2-1 0 0,3 0-4 0 0,13 2-28 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-4-3 1 0 0,6 4-15 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-2 0 0 0,2-30-131 0 0,2 1-1 0 0,14-60 1 0 0,-7 42 61 0 0,136-491-986 0 0,-108 429 741 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-42081.48">1934 2236 6680 0 0,'0'0'505'0'0,"8"14"-314"0"0,-4-6-200 0 0,0 0 0 0 0,0 0 0 0 0,2 11 0 0 0,1-1-27 0 0,0 4-121 0 0,-1-1 0 0 0,0 0 1 0 0,2 38-1 0 0,-3-28 2 0 0,-5 3 514 0 0,-1-34-321 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,2 1-7 0 0,-2-2-14 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1-2 1 0 0,1-1 14 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,0-7 1 0 0,2-19-338 0 0,1 1 0 0 0,2 1 0 0 0,10-38 0 0 0,-13 57 295 0 0,1-3 34 0 0,0 2 0 0 0,1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,11-12 0 0 0,-15 22 5 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0-16 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1-1 1 0 0,0 2 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,0 1-1 0 0,-4 6 261 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 0-1 0 0,-13 13 1 0 0,0 0 22 0 0,-9 4-3075 0 0,21-15-276 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-41331.01">2187 2151 6968 0 0,'-5'-4'688'0'0,"12"20"-715"0"0,8 27 0 0 0,-8-22-50 0 0,-5-11 111 0 0,1-1-1 0 0,-1 2 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,-4 11 1 0 0,3-7 351 0 0,2-11-335 0 0,1 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,-2 3-1 0 0,4-6-183 0 0,0-22-1004 0 0,1 16 1043 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 2 1 0 0,0-2-1 0 0,4-6 0 0 0,-6 10 104 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,3 0 0 0 0,10 5 241 0 0,1 1-1 0 0,13 10 1 0 0,-15-11 26 0 0,0 2-1 0 0,26 9 1 0 0,-36-16-443 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,1-1 0 0 0,2-1 0 0 0,3 0-2490 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-40990.69">2173 2403 12528 0 0,'-8'-7'600'0'0,"8"2"-256"0"0,0 1 8 0 0,3-3-280 0 0,2 0-72 0 0,3-2 0 0 0,3-2 0 0 0,5 2-216 0 0,2-6-56 0 0,0 2-16 0 0,4-2-4992 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-39541.04">2168 2393 3728 0 0,'8'-6'232'0'0,"69"-52"212"0"0,-22 16-80 0 0,-38 28 244 0 0,-1-1 0 0 0,23-28 0 0 0,-37 41-609 0 0,-2 2 1 0 0,1-1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 57 0 0,-1 2-73 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,-15 17-536 0 0,10-9 261 0 0,-20 17-772 0 0,17-16-609 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-38477.4">2840 1923 1408 0 0,'0'0'136'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-38071.73">2798 1847 6968 0 0,'0'0'528'0'0,"11"-9"-336"0"0,-8 8-205 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,5 0-1 0 0,-6 0 7 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1 2 103 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,-2 5 0 0 0,2-5-24 0 0,-36 186 2552 0 0,-15 297-2401 0 0,16 5-361 0 0,27-357 100 0 0,-10 207-117 0 0,-9 127-297 0 0,23-406 104 0 0,2-2-6 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-19849.37">3022 2876 8088 0 0,'0'0'1376'0'0,"2"20"-1088"0"0,-1 36-317 0 0,-1 51-68 0 0,-1-85 98 0 0,1-16 5 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-4 10 0 0 0,5-15-2 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-6-9 317 0 0,6 10-313 0 0,-3-8 82 0 0,1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,1 0 1 0 0,1-13-1 0 0,2-3-83 0 0,13-43 1 0 0,6 4-271 0 0,-20 56 249 0 0,0-1 1 0 0,1 1-1 0 0,0 1 1 0 0,1 0-1 0 0,0-1 1 0 0,6-6-1 0 0,-9 12 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,3-2 1 0 0,-5 3 8 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,2 0 0 0 0,0 2 1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2 2 0 0 0,-1 5 107 0 0,-1-1 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 1 0 0,-10 16-1 0 0,-28 41-233 0 0,37-52-893 0 0,3-7-2813 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-19495.34">3334 2914 10280 0 0,'0'0'230'0'0,"-6"-3"565"0"0,4 0-703 0 0,-2 0-63 0 0,3 2 321 0 0,-1 4-383 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-2 5 0 0 0,3-7 25 0 0,-5 14-230 0 0,2 1 1 0 0,-4 29 0 0 0,5-30 99 0 0,-1 21-526 0 0,1-17 290 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-19126.86">3424 3069 9416 0 0,'0'0'706'0'0,"1"1"-482"0"0,0-1-205 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 1-1 0 0,23-11 791 0 0,-6 2-508 0 0,-15 7-278 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,6-6 0 0 0,-7 5-27 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0-1 1 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,2-8-1 0 0,-3 8 2 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,-2-2-1 0 0,-4-2 80 0 0,1 0 0 0 0,-13-6 1 0 0,12 7 288 0 0,0 0 1 0 0,-12-10-1 0 0,18 13-289 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-2-3 1 0 0,3 4-230 0 0,0-1 60 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,2-3 0 0 0,1 2 11 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,8-2 0 0 0,5-4-717 0 0,-8 4 346 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-17970.38">3921 2700 7200 0 0,'0'-1'22'0'0,"2"-7"170"0"0,-1 0 1 0 0,1-1 0 0 0,0 1-1 0 0,6-14 1136 0 0,-7 22-1309 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,3 11 102 0 0,-1 1-1 0 0,0 0 0 0 0,-1 14 1 0 0,-1 50-40 0 0,-5 178 318 0 0,5-220-3389 0 0,2-25-372 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-17600.59">4060 2621 10208 0 0,'0'0'298'0'0,"3"15"116"0"0,12 45-125 0 0,9 74 0 0 0,-1-1 37 0 0,-22-129-230 0 0,1 1-543 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,-1 10-1 0 0,-4-5-830 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-17245.95">3732 2893 11256 0 0,'5'-14'857'0'0,"-3"11"-816"0"0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,5-4 0 0 0,30-13-71 0 0,56-16 6 0 0,-78 30-56 0 0,-1 0-1 0 0,1 2 0 0 0,0 0 0 0 0,20 0 0 0 0,-28 1-612 0 0,0 0 0 0 0,0 0 0 0 0,8-2 0 0 0,-12 2 515 0 0,8-2-924 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-16876.95">3861 2986 14856 0 0,'11'-7'1122'0'0,"43"-25"-613"0"0,-43 26-401 0 0,0 0 0 0 0,0 1 0 0 0,1 0-1 0 0,-1 1 1 0 0,24-4 0 0 0,-13 2 25 0 0,225-52-441 0 0,-232 55-234 0 0,21-4-360 0 0,-12 3-3619 0 0,-10 4-225 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="55144.3">4357 7993 6968 0 0,'0'0'337'0'0,"13"8"46"0"0,-8-6-116 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,4 5 0 0 0,-5-5-18 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,6 1 1 0 0,5-1-92 0 0,1-1 1 0 0,-1-1 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,1-2 0 0 0,-1 0 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1-1 0 0 0,16-9 0 0 0,10-8 236 0 0,-1-1 1 0 0,54-44-1 0 0,-72 49-255 0 0,0 0 0 0 0,-1-1-1 0 0,-1-1 1 0 0,-1-1 0 0 0,-1-1-1 0 0,17-30 1 0 0,-15 19-86 0 0,-1-1-1 0 0,-2-1 1 0 0,22-72-1 0 0,-33 86-153 0 0,0 0-1 0 0,-1 0 0 0 0,-2 1 0 0 0,0-2 0 0 0,-3-43 0 0 0,-2 37 47 0 0,-1 0 0 0 0,-1 1 0 0 0,-2 0 0 0 0,-12-32-1 0 0,11 35 126 0 0,-2 1-1 0 0,-1 1 0 0 0,0-1 1 0 0,-2 2-1 0 0,-1-1 0 0 0,0 2 0 0 0,-2 0 1 0 0,0 0-1 0 0,-23-19 0 0 0,-7 1 94 0 0,-2 2-1 0 0,-77-45 1 0 0,96 64-195 0 0,-12-6 21 0 0,-45-18 0 0 0,-3-2 109 0 0,67 32-177 0 0,-121-69 3 0 0,118 65 117 0 0,1-2-1 0 0,0-1 1 0 0,-31-31-1 0 0,36 30 16 0 0,2 0 0 0 0,0-2 0 0 0,1 0 0 0 0,1 0 0 0 0,1-2 0 0 0,1 1 0 0 0,1-1 0 0 0,-14-44 0 0 0,22 53-66 0 0,1-1 0 0 0,0 1 0 0 0,2-1 0 0 0,0 1-1 0 0,0 0 1 0 0,1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,7-27 0 0 0,-1 12-41 0 0,1 2 0 0 0,1 0 0 0 0,29-56 1 0 0,-14 43-17 0 0,1 1 0 0 0,39-47 0 0 0,71-69-57 0 0,-117 135 130 0 0,43-39-67 0 0,97-79 0 0 0,-97 91-2 0 0,3 3 0 0 0,2 3-1 0 0,2 2 1 0 0,93-40-1 0 0,37 8-5238 0 0,-130 53-41 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56240.86">5143 1888 9760 0 0,'-1'-2'16'0'0,"1"1"1"0"0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 2 1 0 0,0-2-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,2-1-1 0 0,4-5 110 0 0,0 0 0 0 0,1 0 0 0 0,8-5 1 0 0,-7 6-92 0 0,37-27-57 0 0,82-43 0 0 0,58-15-51 0 0,-69 35 54 0 0,-66 33 19 0 0,1 2 0 0 0,99-27 0 0 0,-133 43 7 0 0,-1 2 0 0 0,1 0 1 0 0,18 0-1 0 0,-31 3-4 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,7 6 0 0 0,-9-5 8 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-2 6 0 0 0,-1 10 78 0 0,-1-1-1 0 0,0 0 1 0 0,-11 25-1 0 0,14-43-71 0 0,-20 61 154 0 0,1 1 0 0 0,-10 68 0 0 0,28-119-165 0 0,1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,2-1 1 0 0,-1 1 0 0 0,2-1-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0-1 0 0,0-1 1 0 0,8 19 0 0 0,-5-17 0 0 0,1 0 1 0 0,0 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,17 13 0 0 0,-4-7-84 0 0,0 0 1 0 0,0-2-1 0 0,1 0 1 0 0,43 16-1 0 0,-17-12-100 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="128725.23">8862 851 8144 0 0,'-6'-10'809'0'0,"6"7"-788"0"0,11 12-370 0 0,-6 3 311 0 0,-1 0-1 0 0,-1 0 0 0 0,4 21 1 0 0,0 3-1 0 0,-5-30 44 0 0,2 14 187 0 0,1 0 1 0 0,1 0-1 0 0,1 0 1 0 0,1-1-1 0 0,13 23 1 0 0,-2-12 118 0 0,-4-5 121 0 0,19 25 1 0 0,-32-48-362 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 6 1 0 0,-2-8-63 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,-24 2-89 0 0,25-2 80 0 0,-11 0 80 0 0,0-1 0 0 0,-16-4-1 0 0,-12-1 248 0 0,-23-1-16 0 0,-38-1-1617 0 0,100 8 934 0 0,-7 0 501 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="129393.04">9195 1090 5152 0 0,'0'0'116'0'0,"4"-15"664"0"0,-3 12-393 0 0,0 2-191 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 0-181 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,5 20 527 0 0,-5-19-472 0 0,2 6 347 0 0,-1-1 1 0 0,6 16-1 0 0,-6-20-308 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,5 4 0 0 0,-5-5-73 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 0-1 0 0,3-1 1 0 0,0-1-119 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,6-6 0 0 0,-1-1-96 0 0,-1-2 0 0 0,0 1 0 0 0,-1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,-1-1 0 0 0,6-21 0 0 0,5-13 503 0 0,-15 46-223 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,2-2 0 0 0,-3 4-81 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 2 0 0 0,6 19 30 0 0,-1 0 1 0 0,-1 1-1 0 0,-1 0 1 0 0,1 23 0 0 0,-3-23-225 0 0,0 0 0 0 0,2 0 0 0 0,1-1 0 0 0,8 25 0 0 0,-9-39-428 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="129979.17">9640 1035 11376 0 0,'0'0'1133'0'0,"-4"16"-1016"0"0,2-4-134 0 0,0 1-1 0 0,2 0 1 0 0,0 16-1 0 0,0-16-170 0 0,0-13 178 0 0,0 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,5-5-272 0 0,5-9-49 0 0,3-13 4 0 0,10-28-1 0 0,-16 35 451 0 0,0 0 0 0 0,1 0 0 0 0,23-33-1 0 0,-30 49 6 0 0,1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 2 1 0 0,8-5-1 0 0,-9 5-73 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,4 1 1 0 0,-1 1-13 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1 0 0 0,3 6 0 0 0,1 6 18 0 0,0 0 0 0 0,-2 1 1 0 0,3 18-1 0 0,-3-17-1591 0 0,0-2 0 0 0,7 22 0 0 0,-6-30-2615 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="130669.48">10297 836 11600 0 0,'-3'-16'1253'0'0,"3"15"-1353"0"0,-1 1-613 0 0,-1-1 502 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-4 1-1 0 0,-2 2-247 0 0,0 0 0 0 0,0-1 0 0 0,-10 3 0 0 0,10-3 554 0 0,1-1 0 0 0,-1 1-1 0 0,1 1 1 0 0,-8 3 0 0 0,-2 2 660 0 0,-13 9 687 0 0,27-15-1355 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 4 0 0 0,0-5-66 0 0,1 2 1 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0-1 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 1 0 0,4 4-1 0 0,3 0-33 0 0,0 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 0-1 0 0,11 2 0 0 0,1-1-550 0 0,-1-2 1 0 0,31 0-1 0 0,-29-2-3609 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="131003.6">10730 353 14864 0 0,'0'0'916'0'0,"11"12"-4159"0"0,-8-5 3134 0 0,0 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,1 13 0 0 0,0 44-719 0 0,-2-34 676 0 0,-4 144 160 0 0,0-30-472 0 0,4-111-47 0 0,1 0 0 0 0,10 44-1 0 0,-10-67-3322 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="131341.94">10557 737 14600 0 0,'0'0'330'0'0,"8"-10"797"0"0,-5 8-1110 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,6-2 0 0 0,35-5-167 0 0,-39 8 115 0 0,34-5-33 0 0,0 2-1 0 0,1 2 1 0 0,64 7 0 0 0,-103-6-265 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 1 0 0,3 0-1 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="131711.84">10972 802 15176 0 0,'-6'-7'484'0'0,"5"6"-389"0"0,0 0 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-2-2 0 0 0,2 1-160 0 0,2 16-997 0 0,5 25 0 0 0,-3-20 461 0 0,-1-11 329 0 0,1 8-224 0 0,-1 0-1 0 0,-1-1 0 0 0,0 32 0 0 0,-4 29 558 0 0,7-83-430 0 0,-1-3 176 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="132065.53">11177 911 14368 0 0,'-15'-6'1562'0'0,"9"9"-1493"0"0,4-2-155 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 3 0 0 0,3-3 64 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 4-1 0 0,0-6 30 0 0,-1 1-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,2-1-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,3 0 1 0 0,1 0 42 0 0,0 0 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,4-4 0 0 0,-6 4-77 0 0,0 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 1 0 0 0,1-6 0 0 0,-1 3 64 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 1 0 0 0,-8-12 0 0 0,9 13 37 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-9-3 1 0 0,11 6-200 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 2 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,-2 3 0 0 0,-5 8-1028 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="132891.88">11511 779 15856 0 0,'0'-4'1006'0'0,"4"10"-1106"0"0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 8 0 0 0,0 14-675 0 0,-5 34 0 0 0,1-23 516 0 0,-10 69 259 0 0,13-106 1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,-2 4 0 0 0,2-5 216 0 0,2-10 84 0 0,27-164 466 0 0,-18 129-771 0 0,30-80 0 0 0,-36 115-22 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,9-11 1 0 0,-12 16 19 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 1 0 0,2 0-1 0 0,-4 1 16 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 2 0 0 0,2 5 32 0 0,0 0-1 0 0,-1-2 0 0 0,4 15 1 0 0,51 221 39 0 0,-51-208-602 0 0,-4-15 14 0 0,0-4-6 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="159112.67">802 412 11792 0 0,'-7'-1'417'0'0,"4"0"-361"0"0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,-3 0 0 0 0,5 0-58 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 2-1 0 0,-1 6 12 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 14 0 0 0,-1 4 36 0 0,-2 131-352 0 0,5-101 311 0 0,-1-8-37 0 0,13 97 0 0 0,-13-142 34 0 0,0-3 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 1 0 0 0,-1-2-14 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,4-15-6 0 0,-1 0 0 0 0,0 1 0 0 0,2-29 0 0 0,-1 3 26 0 0,37-273 46 0 0,-41 306-54 0 0,1-12 0 0 0,1 0 0 0 0,10-36 0 0 0,-11 52-241 0 0,0 7 112 0 0,-1 5-81 0 0,-5 62-16 0 0,-3 1 1 0 0,-19 82-1 0 0,18-111 112 0 0,-45 204 54 0 0,35-168 104 0 0,10-44 24 0 0,-20 49 0 0 0,-5-9 969 0 0,33-73-1025 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-2-7 184 0 0,1-8-269 0 0,17-119-1548 0 0,-2 13-997 0 0,-12-170-2244 0 0,-2 190 9556 0 0,5 105-3546 0 0,1 3-892 0 0,-3 0-339 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 10 0 0 0,3 20-3256 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="159733.47">729 280 12816 0 0,'-10'-3'183'0'0,"1"0"0"0"0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-19 1 0 0 0,23 0-211 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,-5 6 0 0 0,-7 9-177 0 0,2 1 0 0 0,1 0-1 0 0,-12 23 1 0 0,-32 68-817 0 0,25-44 513 0 0,-18 36 193 0 0,-47 129 0 0 0,80-178 493 0 0,2 1 0 0 0,3-1 0 0 0,2 2 0 0 0,-6 82 0 0 0,16-104-166 0 0,1-1 1 0 0,1 1-1 0 0,10 48 0 0 0,-7-61-9 0 0,1-1-1 0 0,1 0 0 0 0,0-1 1 0 0,2 0-1 0 0,0 0 0 0 0,22 34 1 0 0,-19-36 6 0 0,0 0 0 0 0,2-2 0 0 0,0 1 0 0 0,1-1 0 0 0,1-2 1 0 0,0 0-1 0 0,25 18 0 0 0,-30-24-8 0 0,1-1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-2 0 0 0,1 1-1 0 0,-1-2 1 0 0,1 0-1 0 0,-1 0 1 0 0,16-2 0 0 0,-11-1 0 0 0,0 0 0 0 0,0-2 0 0 0,0 0 0 0 0,0-1 1 0 0,-1-1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 0 1 0 0,16-12-1 0 0,-2-2-49 0 0,-1 0 0 0 0,0-3 0 0 0,41-48 0 0 0,-36 33-96 0 0,-2 0-1 0 0,-2-2 0 0 0,27-53 0 0 0,-20 23-35 0 0,34-97 0 0 0,-51 109 820 0 0,-2 1 0 0 0,-4-2 1 0 0,-2-1-1 0 0,-2 2 0 0 0,-4-3 0 0 0,-3-114 1 0 0,-5 134-411 0 0,-2-1 0 0 0,-19-84 1 0 0,17 101-223 0 0,-2 1-1 0 0,0 1 1 0 0,-2 0 0 0 0,-1 0 0 0 0,-1 2 0 0 0,-16-25 0 0 0,24 42-7 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 2 0 0 0,-14-7 0 0 0,10 7 0 0 0,0-1 0 0 0,0 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-18 2 0 0 0,-1 2 0 0 0,0 2 0 0 0,1 1 0 0 0,0 1 0 0 0,0 2 0 0 0,-38 17 0 0 0,14-3-455 0 0,1 3 1 0 0,2 3 0 0 0,1 0-1 0 0,1 4 1 0 0,2 1 0 0 0,2 3-1 0 0,-69 70 1 0 0,55-42-471 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="161323.91">7050 1337 7920 0 0,'-7'-3'195'0'0,"5"2"-34"0"0,-1 0 1 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,-5-1 0 0 0,18 1-62 0 0,0-1 0 0 0,18-5 1 0 0,-7 2-50 0 0,-4 1 10 0 0,0 2-1 0 0,1 0 1 0 0,-1 1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 1-1 0 0,0 1 1 0 0,0 1 0 0 0,17 7 0 0 0,-29-11-61 0 0,0 1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,6 8 0 0 0,-9-9 7 0 0,1-1 0 0 0,-1 2 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2 2 0 0 0,-4 10 63 0 0,-1-1-1 0 0,-1 1 0 0 0,0-2 1 0 0,-1 1-1 0 0,0-1 1 0 0,-15 16-1 0 0,11-15 177 0 0,2 1-1 0 0,0 0 1 0 0,-17 33-1 0 0,23-37-159 0 0,0 0-1 0 0,1 1 1 0 0,0-1-1 0 0,-2 18 1 0 0,5-24-56 0 0,0 1 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,2-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,5 10 1 0 0,-4-11-86 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,7 4 0 0 0,-8-7 9 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,3-2 0 0 0,16-6-655 0 0,-4-1-4 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="162055.6">7000 1248 13616 0 0,'-10'-3'68'0'0,"0"1"0"0"0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 2 0 0 0,0-1 0 0 0,0 1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,0 1 0 0 0,0 0 1 0 0,-16 12-1 0 0,10-3-136 0 0,1 0 1 0 0,0 1-1 0 0,1 1 1 0 0,0 0-1 0 0,2 0 1 0 0,0 1-1 0 0,0 0 1 0 0,2 1-1 0 0,-14 37 1 0 0,10-16 24 0 0,1 0 1 0 0,3 1-1 0 0,-9 77 1 0 0,14-71-3 0 0,2 0 0 0 0,8 81-1 0 0,-3-99 31 0 0,2 0 0 0 0,0-1-1 0 0,2-1 1 0 0,1 1-1 0 0,22 48 1 0 0,-25-65 16 0 0,1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1-2 0 0 0,1 2 0 0 0,0-1 1 0 0,1 0-1 0 0,0-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,17 7 0 0 0,-8-5 158 0 0,1-2 0 0 0,0 0 0 0 0,0-1-1 0 0,1-1 1 0 0,-1-2 0 0 0,44 2 0 0 0,-22-5 59 0 0,-1-2 0 0 0,1-1 0 0 0,76-19 0 0 0,-90 15-199 0 0,0-1 0 0 0,0-1 0 0 0,-2-2 0 0 0,1-1 0 0 0,-2-1 0 0 0,34-22 0 0 0,-42 23-6 0 0,-1-2 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 0 1 0 0,20-28-1 0 0,-18 20-28 0 0,-1-2 1 0 0,-1-1 0 0 0,17-41-1 0 0,-22 40 57 0 0,-1 2 0 0 0,-2-3-1 0 0,0 1 1 0 0,-2-1 0 0 0,-2 1-1 0 0,0-1 1 0 0,-3-54 0 0 0,-3 43 198 0 0,-2 0 0 0 0,-1 1 0 0 0,-2 0 0 0 0,-2 0 0 0 0,-18-42-1 0 0,18 57-124 0 0,-1 0-1 0 0,-1 2 0 0 0,0-1 0 0 0,-2 2 0 0 0,-1 0 0 0 0,-1 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1 1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,-1 1 1 0 0,0 2-1 0 0,-1 0 0 0 0,-1 2 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 1 0 0 0,0 2 0 0 0,-1 0 0 0 0,0 1 0 0 0,-35-4 0 0 0,29 7-229 0 0,1 1-1 0 0,-1 2 0 0 0,0 2 1 0 0,1 0-1 0 0,-1 2 0 0 0,-58 13 1 0 0,64-9-1863 0 0,1 1 1 0 0,-38 18 0 0 0,20-5-3905 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="163336.04">870 7976 13104 0 0,'0'0'1'0'0,"-22"-8"933"0"0,21 8-925 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,2-1 0 0 0,7-4 13 0 0,1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,0 2-1 0 0,11-3 1 0 0,-4 0 62 0 0,1 0 63 0 0,21-5 158 0 0,72-6 0 0 0,-100 14-274 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 1 0 0 0,1 0 0 0 0,18 8 0 0 0,-27-10-50 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,0 6 0 0 0,0 7-92 0 0,-1 1 0 0 0,-1-1-1 0 0,-5 26 1 0 0,3-25 67 0 0,-7 21 16 0 0,9-31 20 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 10-1 0 0,3-15 6 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0-1 0 0 0,3 2 1 0 0,6 3-17 0 0,1-2 0 0 0,-1 1 0 0 0,1-2 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,17-1 0 0 0,86-9-179 0 0,-84 4 173 0 0,137-21-147 0 0,-74 10 15 0 0,-53 10-181 0 0,-40 5 342 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-8 10 366 0 0,-3-1 160 0 0,0 0 0 0 0,-12 8 0 0 0,9-8-41 0 0,-16 15 0 0 0,-139 117 1060 0 0,71-61-1218 0 0,42-28 29 0 0,33-30-2626 0 0,10-9-1277 0 0,0 0-2327 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="164396.16">1267 7185 18287 0 0,'-44'4'687'0'0,"1"2"0"0"0,-80 23 0 0 0,106-24-726 0 0,1 1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 2-1 0 0,0-1 1 0 0,0 1 0 0 0,1 1 0 0 0,0 1 0 0 0,1 0 0 0 0,-16 17 0 0 0,-7 15-360 0 0,-53 82 0 0 0,-21 57-633 0 0,69-110 611 0 0,-80 168-866 0 0,17 10 896 0 0,67-159 386 0 0,4-11-15 0 0,4 3 1 0 0,4 0 0 0 0,4 2 0 0 0,-16 124 0 0 0,34-177 11 0 0,2 2 1 0 0,0-1 0 0 0,3 1 0 0 0,1-1 0 0 0,1-1 0 0 0,1 1 0 0 0,2 0 0 0 0,20 55 0 0 0,-18-66 6 0 0,2 1 0 0 0,0-1 0 0 0,1 0 1 0 0,1 0-1 0 0,1-1 0 0 0,1-1 0 0 0,1-2 0 0 0,0 1 0 0 0,2-1 0 0 0,0 0 1 0 0,1-2-1 0 0,27 18 0 0 0,-25-19 1 0 0,1-2 1 0 0,0-1-1 0 0,1-1 1 0 0,1-2-1 0 0,-1 1 1 0 0,2-2-1 0 0,-1-1 1 0 0,1-1-1 0 0,1-1 1 0 0,-1-1-1 0 0,1-1 1 0 0,-1-2-1 0 0,37-1 1 0 0,-27-4 51 0 0,0-1 0 0 0,0-1 1 0 0,-1-2-1 0 0,0-2 1 0 0,50-19-1 0 0,-43 10 7 0 0,-2-1 1 0 0,0-1-1 0 0,-2-3 1 0 0,36-27 0 0 0,-50 33-28 0 0,123-99 294 0 0,-109 84-114 0 0,58-67 0 0 0,-23 11 107 0 0,-5-4-1 0 0,-4-2 1 0 0,-5-3 0 0 0,-3-2-1 0 0,60-155 1 0 0,24-178 327 0 0,-117 338-973 0 0,-4-3 0 0 0,9-156 0 0 0,-25 219 234 0 0,-2 0-1 0 0,-2 2 1 0 0,-1-2-1 0 0,-9-42 0 0 0,8 62 92 0 0,0 1 0 0 0,0 0 0 0 0,-2 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,-15-14-1 0 0,13 14-25 0 0,-1 1 0 0 0,-1 2-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 2 1 0 0,0 0-1 0 0,-18-6 1 0 0,13 7-88 0 0,-1 0 0 0 0,-1 2 0 0 0,1 0 1 0 0,-43-1-1 0 0,9 5-14 0 0,1 3 0 0 0,0 2 0 0 0,1 2 0 0 0,-70 19 0 0 0,40-2 76 0 0,-157 67-1 0 0,142-44 76 0 0,3 4 0 0 0,-145 104 0 0 0,109-56-178 0 0,-125 124 0 0 0,-42 104-2166 0 0,226-235-2825 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="175390.74">3014 3770 7168 0 0,'-1'0'208'0'0,"0"0"1"0"0,17 7-109 0 0,-4 0-105 0 0,-7-5 14 0 0,1 0 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,7-3 1 0 0,9-4 188 0 0,-9 3-19 0 0,-1 0 0 0 0,16-8 0 0 0,-24 10-152 0 0,1 0 0 0 0,-1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,3-5 1 0 0,-4 6 30 0 0,1-1 0 0 0,-2 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1-4 1 0 0,0 5-8 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-6-3 0 0 0,-14-4 21 0 0,0 1-1 0 0,-1 1 1 0 0,0 1 0 0 0,-39-5 0 0 0,40 8-55 0 0,1 1 0 0 0,-9-2 45 0 0,29 3-57 0 0,1 1 0 0 0,-1-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-2-2 0 0 0,2 1 19 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 2 1 0 0,0-2-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,1-3 0 0 0,6-5-156 0 0,-1 1 1 0 0,2-1 0 0 0,11-9-1 0 0,-16 14 82 0 0,17-12-1182 0 0,-11 6-2474 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="176046.37">3308 3519 14896 0 0,'-3'-3'36'0'0,"1"2"35"0"0,1-1-1 0 0,-1 2 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-4 1-1 0 0,4 0-62 0 0,2 0-8 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 0-73 0 0,-1 14-408 0 0,5 0 357 0 0,5 31-158 0 0,-2-1 1 0 0,1 46 0 0 0,-7-75 120 0 0,1-11 126 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,-3 5-1 0 0,4-7 50 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-9-11 120 0 0,6 6-121 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-2-13 1 0 0,-1-46-36 0 0,4 47 19 0 0,0 7-9 0 0,0 0 1 0 0,1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 2 0 0 0,1-2 0 0 0,1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,7-13 0 0 0,-8 17-116 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,1-1 0 0 0,10-8 1 0 0,-13 11 54 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,5 1 0 0 0,-8 0 35 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,1 2 1 0 0,-1-1 48 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-2 2-1 0 0,-57 88 667 0 0,58-89-569 0 0,0-1-1 0 0,0 2 1 0 0,0-2 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,0 1 0 0 0,0 3 0 0 0,0-4-98 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,4 1 1 0 0,-1 0-178 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,2-1 0 0 0,-2 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,8-4 1 0 0,-2 2-603 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="176597.45">3737 3361 13072 0 0,'-34'-29'1432'0'0,"33"28"-1556"0"0,12 18-388 0 0,-3 15 508 0 0,-1 0 0 0 0,2 39 1 0 0,2 10-122 0 0,-4-33-104 0 0,-3-21-763 0 0,8 35 1 0 0,-6-49-3201 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="176962.9">3718 3304 13416 0 0,'-4'-3'288'0'0,"-2"1"64"0"0,4-1 480 0 0,10 1-832 0 0,-1 0-128 0 0,6 0-48 0 0,6 0-8 0 0,-1 2 0 0 0,0-3-80 0 0,6-2-24 0 0,-2 1 0 0 0,1-1-3320 0 0,0 5-664 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="176963.9">3703 3547 9416 0 0,'-5'-5'976'0'0,"10"5"-976"0"0,3 3 0 0 0,-1-3 0 0 0,7-3 0 0 0,-1 3-96 0 0,3-2 0 0 0,2 2 0 0 0,0 0-184 0 0,0-2-32 0 0,4-1-8 0 0,-4-1-3392 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="177548.69">3968 3299 13344 0 0,'-52'-55'664'0'0,"64"102"-729"0"0,-1 0 1 0 0,7 70-1 0 0,-2-7-101 0 0,-8-27 177 0 0,-2-17-1014 0 0,-4-59 707 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="178599.56">4262 3551 15000 0 0,'-23'-12'824'0'0,"-35"-21"-1"0"0,52 28-829 0 0,4 4-56 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,-2 0 0 0 0,-1 0-375 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,-7 2 1 0 0,10-1 250 0 0,-1 0 204 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-7 2 0 0 0,9-3 8 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 2 0 0 0,1 4-28 0 0,1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,6 10-1 0 0,-7-13 18 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,0-2 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,5 1 1 0 0,-7-1 13 0 0,1-1 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,2-2-1 0 0,0 0-3 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-8 0 0 0,-2 9 141 0 0,0-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,-5-8 942 0 0,9 24-853 0 0,66 143-659 0 0,-59-135 140 0 0,-7-14-204 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,7 5 0 0 0,0-7-1163 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="179013.94">4575 3343 11376 0 0,'0'0'256'0'0,"-16"5"717"0"0,10-3-959 0 0,0 1 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1 0 0 0,0 1-1 0 0,0-1 1 0 0,-7 10 0 0 0,0 0-20 0 0,1 1-1 0 0,-12 23 1 0 0,-9 13 936 0 0,30-48-848 0 0,0-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 1 0 0,-1 5-1 0 0,-1 5 59 0 0,2-9-128 0 0,0-3 276 0 0,14-13 497 0 0,-7 6-842 0 0,-1-1 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,8-15 0 0 0,-4 1-388 0 0,7-22 1 0 0,-13 37 318 0 0,-1 1 0 0 0,0-1 0 0 0,1-10 0 0 0,-2 16 808 0 0,-2 5 173 0 0,0 2-751 0 0,1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,2 8-1 0 0,-1 8-38 0 0,5 124 123 0 0,17 166 109 0 0,-18-258-306 0 0,5 36 81 0 0,3-1 0 0 0,5 0 0 0 0,48 146 0 0 0,-49-184-4901 0 0,-10-27-465 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="202839.22">6073 3851 7136 0 0,'-8'9'200'0'0,"5"-4"48"0"0,0 0-248 0 0,1-1 0 0 0,2 3 0 0 0,0-2 0 0 0,0-1 200 0 0,2 1-8 0 0,1 2 0 0 0,0-2 0 0 0,2-1-192 0 0,3-2 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1-104 0 0,0-1-16 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="205449.54">6005 3352 7792 0 0,'-4'2'83'0'0,"0"0"0"0"0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-4 5 0 0 0,6-7-65 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,2 1 0 0 0,-1 0-18 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,5 1 0 0 0,29-2-128 0 0,-26 0 64 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37141.14">11271 3846 5160 0 0,'0'0'1581'0'0,"-3"10"-866"0"0,3 7-420 0 0,0-4-165 0 0,0 0 0 0 0,2 18 0 0 0,-1-28-91 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,3 4 1 0 0,-5-6 40 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 1 0 0,6-5 234 0 0,0 1 0 0 0,11-11-1 0 0,-15 12-390 0 0,42-32 42 0 0,-27 22 19 0 0,28-27 1 0 0,-43 37-7 0 0,15-13-1594 0 0,-2-2-1 0 0,23-33 1 0 0,-37 48-1329 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37682.35">11137 4302 7344 0 0,'0'0'11'0'0,"0"0"0"0"0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,0 0 0 0 0,11-10 329 0 0,-12 11-333 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,13 9 424 0 0,-3-2-140 0 0,-8-5-200 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 1 1 0 0,1 3-1 0 0,-1-3-86 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,6 6-1 0 0,-7-8 33 0 0,-1-1-19 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,6 5 115 0 0,-8-5-100 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 1 0 0,12-6 569 0 0,-10 5-567 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,4-4 1 0 0,182-167 224 0 0,-166 150-254 0 0,57-45-338 0 0,-19 16-341 0 0,33-27-1431 0 0,-49 42 1017 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="40299.53">10885 5886 7920 0 0,'-1'-1'112'0'0,"-9"-12"370"0"0,7 9 12 0 0,6 6 331 0 0,0 1-767 0 0,-1 0-1 0 0,1 1 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 5 1 0 0,3 11 161 0 0,-1-7-137 0 0,12 33 181 0 0,-14-43-191 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,6 5 0 0 0,-7-7 17 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,4-1-1 0 0,5-2 465 0 0,22-7 0 0 0,-32 10-524 0 0,35-15 489 0 0,0-2 1 0 0,46-28 0 0 0,-60 32-710 0 0,20-12-272 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="46530.04">11493 3288 9416 0 0,'-36'-10'2668'0'0,"40"10"-2520"0"0,10 0-148 0 0,-9-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,7 3 0 0 0,-6-2-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,4 6-1 0 0,2 5 46 0 0,13 23-1 0 0,-7-9 134 0 0,6 8 119 0 0,-13-20-285 0 0,1 1 1 0 0,1-2-1 0 0,20 23 1 0 0,50 48 674 0 0,-139-153 249 0 0,-17-3-930 0 0,-28-29 60 0 0,67 64-96 0 0,-61-43 0 0 0,71 51-57 0 0,29 25-37 0 0,6 2 15 0 0,10 4-34 0 0,-11 0 139 0 0,0 1 0 0 0,0-1 0 0 0,9 11 0 0 0,9 5 7 0 0,58 44 7 0 0,-65-52-14 0 0,0 0 0 0 0,0-2 0 0 0,1 0-1 0 0,0-1 1 0 0,27 9 0 0 0,-42-18-12 0 0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,7-2 0 0 0,-11 2 60 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,2-3 0 0 0,-3 2-22 0 0,-1 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,-3-8 65 0 0,-1 1 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,-11-5-1 0 0,-10-7-36 0 0,-38-18 0 0 0,33 19-57 0 0,-32-13-233 0 0,-9-5-178 0 0,71 34 343 0 0,3 1-36 0 0,11 11-467 0 0,-4-6 556 0 0,0 1 0 0 0,0 0 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,5 8 1 0 0,16 15-47 0 0,19 22 12 0 0,-31-34 86 0 0,23 22 1 0 0,35 33-55 0 0,-40-39 412 0 0,-37-52 202 0 0,-7-1-455 0 0,-1 0 1 0 0,-1 1-1 0 0,-1 0 1 0 0,-32-31-1 0 0,-13-17-383 0 0,-19-28-71 0 0,38 53 82 0 0,39 41 213 0 0,1 0 16 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 7 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 17-116 0 0,-1-16 95 0 0,3 20-41 0 0,2 0 0 0 0,0 0 1 0 0,1 0-1 0 0,1 0 1 0 0,16 29-1 0 0,1-4 47 0 0,35 53 0 0 0,-46-81 78 0 0,0-2 1 0 0,1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,1-1 0 0 0,1 0-1 0 0,35 22 1 0 0,-52-36-52 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,-2-9 446 0 0,-11-13 235 0 0,-48-46-209 0 0,13 18-658 0 0,24 23 101 0 0,11 15 168 0 0,-14-21-1 0 0,-75-114-411 0 0,91 138 299 0 0,10 9 10 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1-3-1 0 0,1 5-50 0 0,7 16-210 0 0,26 31 81 0 0,39 42 1 0 0,-66-83 199 0 0,0-2 1 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,13 3 0 0 0,-13-4-122 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,6-2 0 0 0,-1-1-1613 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="47304.01">11913 3034 13104 0 0,'-2'-1'72'0'0,"0"0"0"0"0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-3 1 1 0 0,0 0-39 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,-7 4 0 0 0,-2 4-92 0 0,0 1 0 0 0,1 0 0 0 0,-16 20 0 0 0,27-31 59 0 0,-156 213-557 0 0,-3 2-282 0 0,21-35 733 0 0,128-166 104 0 0,61-63-62 0 0,203-241 812 0 0,-184 207-462 0 0,124-114 0 0 0,-181 188-382 0 0,-8 7-300 0 0,-8 8-264 0 0,-6 7 327 0 0,-1-1 1 0 0,-1 0-1 0 0,-1-1 0 0 0,-13 10 0 0 0,-59 40-116 0 0,51-39 445 0 0,-41 36 0 0 0,-87 73 148 0 0,32-28 1471 0 0,111-84-1099 0 0,18-19-420 0 0,21-6 238 0 0,0-4-272 0 0,1-1 1 0 0,-1-1 0 0 0,28-20 0 0 0,51-46-98 0 0,-31 20 47 0 0,-15 16-54 0 0,95-96 0 0 0,-120 103 162 0 0,-26 33-107 0 0,0-2 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-6 1 0 0,-1 8-14 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,-13 1-10 0 0,1 4 19 0 0,0 0 1 0 0,0 1-1 0 0,0 0 0 0 0,1 1 1 0 0,-17 12-1 0 0,6-3-54 0 0,-33 35 0 0 0,34-29-157 0 0,-27 36-1 0 0,22-20-3370 0 0,6-6-803 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="48520.29">11019 5928 6240 0 0,'-10'-15'392'0'0,"2"4"-64"0"0,3 2 496 0 0,-1 1 0 0 0,0 0 1 0 0,-8-9-1 0 0,4 7 791 0 0,0 0 0 0 0,-13-21 0 0 0,22 31-1578 0 0,0-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,2 0 0 0 0,-2 1-40 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,7 6 2 0 0,-1-1 1 0 0,0 2 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,4 10 0 0 0,28 70 39 0 0,-27-60 9 0 0,48 102 125 0 0,3 8-8 0 0,-61-133-126 0 0,-1-5-27 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,2 2-1 0 0,-1-3 500 0 0,-7-4-82 0 0,-7-7-288 0 0,0 0 1 0 0,-14-17-1 0 0,12 12-87 0 0,-15-17-13 0 0,1-2-1 0 0,2-1 0 0 0,2-1 1 0 0,1-2-1 0 0,-30-66 0 0 0,42 80-28 0 0,-2-6-51 0 0,-24-37-1 0 0,32 61 42 0 0,4 11-12 0 0,3 9-58 0 0,10 29-15 0 0,34 75 1 0 0,-34-93 83 0 0,1 0 1 0 0,2-1-1 0 0,0-1 1 0 0,23 28-1 0 0,-25-36-141 0 0,1-1 0 0 0,0 0 0 0 0,1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,24 13 0 0 0,-23-17-699 0 0,-1-4-38 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="49900.09">11121 5916 8144 0 0,'9'-7'617'0'0,"76"-79"2931"0"0,-83 84-3441 0 0,1-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1-3-1 0 0,0 1 111 0 0,-2 4-211 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,-3 1-8 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,-3 3-1 0 0,-9 6-65 0 0,-33 23-132 0 0,1 2 0 0 0,2 2 0 0 0,-44 48 0 0 0,55-51 418 0 0,-37 42 253 0 0,61-68-553 0 0,-2 6 38 0 0,13-16 49 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,12 2 67 0 0,-5-2-51 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,9-4 0 0 0,40-23-22 0 0,-52 28 2 0 0,23-15-36 0 0,129-80 354 0 0,-132 79-243 0 0,-1 0 0 0 0,-1 0 0 0 0,-1-2 0 0 0,28-34 1 0 0,-38 40-51 0 0,-1 3-13 0 0,12-20 0 0 0,-19 28-9 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0-3-1 0 0,0 5-6 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1-21 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,-3 1 0 0 0,-2 0-73 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-8 3 1 0 0,-6 4 12 0 0,1 1 1 0 0,0 0 0 0 0,1 2 0 0 0,-25 20-1 0 0,-60 64-420 0 0,3 13 262 0 0,-18 20 79 0 0,98-109 249 0 0,2 1 0 0 0,-23 34 1 0 0,41-55-89 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,12 0-61 0 0,13-10-47 0 0,-25 10 108 0 0,22-11 21 0 0,-1-2 1 0 0,0-1 0 0 0,24-20 0 0 0,-8 6 87 0 0,236-164 1188 0 0,-164 118-1102 0 0,-84 56-146 0 0,89-65-61 0 0,-96 69-177 0 0,0-2-1 0 0,-2-1 1 0 0,30-36 0 0 0,-45 51 182 0 0,1 1 1 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-3-1 0 0,-1 5 15 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 0-4 0 0,1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,-1 0 0 0 0,-7 1 11 0 0,0 0 1 0 0,1 0-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 1 1 0 0,0 0-1 0 0,-9 4 1 0 0,0 2 24 0 0,0 0 1 0 0,-22 16-1 0 0,-37 31-76 0 0,3 3-1 0 0,2 3 1 0 0,-89 101 0 0 0,80-76-265 0 0,-71 82-611 0 0,21-26 338 0 0,112-122 389 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="51024.93">11232 3888 5496 0 0,'0'0'417'0'0,"-1"0"-285"0"0,-2-2-79 0 0,2 1 93 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-131 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 9 96 0 0,1-1 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,0 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,7 14-1 0 0,-8-21-46 0 0,1 1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,5 3 1 0 0,-6-5-1 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-2 0 0 0,20-11 187 0 0,16-15-244 0 0,-1-2 1 0 0,-1-1-1 0 0,-1-3 0 0 0,-2 0 0 0 0,-1-1 0 0 0,46-71 1 0 0,-71 95-382 0 0,1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,12-10 0 0 0,-13 15-3345 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="51381.98">11208 4302 9296 0 0,'0'0'16'0'0,"0"-1"0"0"0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1-1-3 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,6 9 342 0 0,1 1 44 0 0,0 0 0 0 0,5 10 0 0 0,-4-1-399 0 0,0 0 0 0 0,15 23 0 0 0,1 10 328 0 0,-12-35 910 0 0,2-15-734 0 0,-13-2-500 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1-1 0 0 0,15-20 58 0 0,-12 15-48 0 0,8-8 33 0 0,-1 1 0 0 0,18-16 0 0 0,8-9-34 0 0,169-179-536 0 0,-175 188 174 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="156482.2">16102 5572 8608 0 0,'0'0'197'0'0,"-6"-2"462"0"0,5 2-661 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,-7 9-270 0 0,6-9 140 0 0,0 1-14 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-4-1 1 0 0,-3 0 171 0 0,0-1 1 0 0,0 0-1 0 0,-12-3 1 0 0,-18-1 468 0 0,27 5-66 0 0,3-1-302 0 0,-1 1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 1 1 0 0,-16 4-1 0 0,-19 13 309 0 0,1 0 0 0 0,-72 47-1 0 0,-51 54 451 0 0,137-98-819 0 0,11-9-11 0 0,0 1 45 0 0,-27 25 1 0 0,41-35-131 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 7 0 0 0,1-5-68 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="158339.17">16218 6300 7632 0 0,'-5'0'54'0'0,"-35"-3"572"0"0,37 3-616 0 0,0 0 1 0 0,0 1-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-6 2-1 0 0,3-1-87 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-11-4 0 0 0,2 0 584 0 0,1 0 1 0 0,0-1-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,-15-14 1 0 0,-4-5 982 0 0,2-2 0 0 0,-47-54 0 0 0,53 56-1093 0 0,-1 0-1 0 0,0 2 0 0 0,-53-37 0 0 0,65 52-399 0 0,-1 0 0 0 0,0 1 0 0 0,0 2 0 0 0,-1-1-1 0 0,-1 1 1 0 0,-27-7 0 0 0,19 7-11 0 0,0 2-1 0 0,-1 1 1 0 0,-42 0 0 0 0,25 2 19 0 0,22 0-27 0 0,0 1 0 0 0,-1 0 0 0 0,-36 7 0 0 0,56-7 14 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1-7 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 2 0 0 0,-16 32-319 0 0,4-14 324 0 0,-1 0 1 0 0,0-1 0 0 0,-1-1 0 0 0,-1-1 0 0 0,-1 0 0 0 0,-30 20 0 0 0,-88 77 38 0 0,-1-1 16 0 0,-92 60 9 0 0,-33 34-54 0 0,-141 98 0 0 0,291-229-25 0 0,-38 28-14 0 0,-377 272 67 0 0,395-286-24 0 0,76-53-121 0 0,-222 162 170 0 0,-137 99-164 0 0,346-251 280 0 0,-230 156 149 0 0,88-42 59 0 0,47-35-386 0 0,-38 41-96 0 0,12 16 359 0 0,29-27-243 0 0,103-102-47 0 0,-179 173 109 0 0,-344 302-214 0 0,384-382 140 0 0,108-83 16 0 0,20-18 31 0 0,-2-2 1 0 0,-81 38-1 0 0,-163 48-39 0 0,262-113 67 0 0,0-3 1 0 0,-2-2 0 0 0,0-3-1 0 0,0-2 1 0 0,-77 2-1 0 0,-190-18 742 0 0,254 3-652 0 0,-109-12 138 0 0,-30-4 451 0 0,24 2-182 0 0,9 0-413 0 0,-32-4 241 0 0,-18-2 536 0 0,118 5-660 0 0,-39-5-100 0 0,-45 21-52 0 0,127 4-122 0 0,22 3-1 0 0,0 0 0 0 0,-54 13 0 0 0,31-4 0 0 0,42-8-17 0 0,1 1-1 0 0,-38 12 0 0 0,-9 11 7 0 0,59-25-15 0 0,1-1 0 0 0,-1 0 1 0 0,-10 0-1 0 0,-3 1-71 0 0,13-1-87 0 0,-7 0 402 0 0,-9-2-3097 0 0,31 7-1763 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="159397.93">6375 10347 9184 0 0,'-12'3'401'0'0,"-12"4"1898"0"0,24 9-2087 0 0,4 2-211 0 0,-2 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-2 0 0 0 0,0-1 0 0 0,-6 24 0 0 0,-26 83 267 0 0,26-103-183 0 0,-1 1 0 0 0,-1 0 0 0 0,-16 25 0 0 0,24-44 11 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,-6 4 1 0 0,10-7-89 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,-2-15 92 0 0,6-58-1092 0 0,22-123 1 0 0,-14 124 657 0 0,-5 28 353 0 0,-2 5-185 0 0,2 1 1 0 0,21-70-1 0 0,-27 107 183 0 0,0-2 41 0 0,0 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,3-3-1 0 0,-4 6 41 0 0,7 7 223 0 0,-6-1-242 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 8 0 0 0,-1 42 568 0 0,-1-41-454 0 0,-3 71 253 0 0,-18 116 0 0 0,-31 81 46 0 0,44-247-248 0 0,-18 51 0 0 0,13-63 324 0 0,9-40-647 0 0,1 1 0 0 0,1-2 1 0 0,0-33-1 0 0,22-270-2013 0 0,-14 248 1603 0 0,12-208-699 0 0,-17 255 2488 0 0,-3 28-632 0 0,-12 107 248 0 0,-1-14-864 0 0,6-38 16 0 0,-25 93 1 0 0,14-91-504 0 0,24-74-105 0 0,-1 0 0 0 0,4-19-1 0 0,2-16-648 0 0,11-54-1548 0 0,-20 100 2682 0 0,6-41-937 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="160457.31">6226 10206 7104 0 0,'0'0'1320'0'0,"-5"-2"1400"0"0,3 4-2688 0 0,0 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 4 0 0 0,2-6-23 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,-1 0-1 0 0,-20 2 21 0 0,20-2-31 0 0,-26 1 37 0 0,-1 2 0 0 0,0 0 1 0 0,1 2-1 0 0,-53 16 0 0 0,53-13 112 0 0,-1-1 0 0 0,-53 6 1 0 0,67-11 239 0 0,0 1 0 0 0,1 1 1 0 0,-23 8-1 0 0,36-12-386 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,3 3 7 0 0,0-1 1 0 0,1 1-1 0 0,-1-2 0 0 0,1 1 0 0 0,4 4 0 0 0,0 2-3 0 0,1 1-7 0 0,0 1 0 0 0,12 10 0 0 0,2 3 0 0 0,101 98 132 0 0,-1 0 120 0 0,-105-104-219 0 0,-2 1 0 0 0,-2 0 1 0 0,0 1-1 0 0,21 43 0 0 0,-29-53 115 0 0,-4-7-16 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 6 0 0 0,-1-9 161 0 0,0-1-418 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,4 3-1344 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink12.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-12-08T23:13:03.265"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1857 7821 9856 0 0,'-5'-3'116'0'0,"1"0"0"0"0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-8 1-1 0 0,-10-2 263 0 0,-10-1-353 0 0,-13-1 153 0 0,18-2 269 0 0,0-1-1 0 0,0 0 1 0 0,1-3 0 0 0,-29-13 0 0 0,19 2-295 0 0,0-2 0 0 0,2 0 0 0 0,-44-40 0 0 0,38 28-156 0 0,2-3 0 0 0,-63-74 1 0 0,-66-72-560 0 0,4 5 468 0 0,57 55 63 0 0,-18-24 51 0 0,96 109-81 0 0,2 0 1 0 0,-31-61 0 0 0,-24-64-55 0 0,79 158 130 0 0,-6-14 14 0 0,0 1 0 0 0,1-1 0 0 0,-8-38 0 0 0,-5-37 35 0 0,17 68-48 0 0,-16-142 24 0 0,19 98 161 0 0,4 0 1 0 0,2 0-1 0 0,4 0 1 0 0,20-81 0 0 0,-7 31-124 0 0,7-24-82 0 0,23-80 60 0 0,-3 9 236 0 0,61-208-50 0 0,-62 268-241 0 0,-17 59-20 0 0,14-49-299 0 0,23-77 166 0 0,22-120 600 0 0,-20-3-427 0 0,-23 58 637 0 0,-5-46-46 0 0,-18 2-112 0 0,-22-37-324 0 0,-5 329-165 0 0,-2-2-1 0 0,-1 2 1 0 0,-16-51-1 0 0,-49-115 140 0 0,2 47-238 0 0,40 80 83 0 0,9 20 64 0 0,-48-146-113 0 0,60 170 54 0 0,5 23 0 0 0,1 0 0 0 0,-7-14 0 0 0,-9-29 2 0 0,11 33 161 0 0,-12-27 0 0 0,-13-20-147 0 0,-17-41-10 0 0,-5-9-85 0 0,14 38 64 0 0,16 31 15 0 0,-36-57 0 0 0,51 96-18 0 0,-1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1 1-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,-25-2 1 0 0,3 0-39 0 0,21 3 58 0 0,0 1 0 0 0,-21-1 0 0 0,25 3-53 0 0,8-1 45 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-5 1 0 0 0,0 2 203 0 0,8-5-251 0 0,0 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1 1 0 0 0,4 7-1011 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink13.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-12-08T23:13:11.818"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">13023 401 17855 0 0,'-43'-36'500'0'0,"-1"1"0"0"0,-2 2-1 0 0,-80-42 1 0 0,90 57-611 0 0,1 2 0 0 0,-2 1 0 0 0,0 2 1 0 0,-1 2-1 0 0,0 1 0 0 0,-42-5 0 0 0,-1 8-293 0 0,-1 2 0 0 0,-129 11 0 0 0,-162 37-962 0 0,109 0 1292 0 0,-310 91 0 0 0,341-60 74 0 0,-349 165 0 0 0,-109 133 18 0 0,526-263 9 0 0,-298 252-1 0 0,309-217-26 0 0,-157 186 1 0 0,-106 208-73 0 0,234-262-153 0 0,-158 325 0 0 0,-85 339-1229 0 0,305-629 1257 0 0,16 7 202 0 0,39-67-26 0 0,-48 371-1 0 0,93-427 197 0 0,8 2-1 0 0,20 299 0 0 0,2-393 151 0 0,5 1 1 0 0,29 106-1 0 0,-22-136-3 0 0,2-2 0 0 0,4 1 0 0 0,54 101-1 0 0,-51-120-79 0 0,3-1-1 0 0,3-1 0 0 0,1-3 0 0 0,63 64 0 0 0,-48-63-4 0 0,3 0-1 0 0,2-4 0 0 0,91 58 0 0 0,-28-34-21 0 0,2-5-1 0 0,146 55 1 0 0,272 72-1174 0 0,-359-134 94 0 0,230 43-1 0 0,-305-83 520 0 0,2-4 0 0 0,0-5 0 0 0,182-8 0 0 0,-188-10 412 0 0,-1-4 0 0 0,144-38 0 0 0,-120 15 163 0 0,180-78 0 0 0,188-139 272 0 0,-28-51 91 0 0,-253 144 577 0 0,267-258 0 0 0,-177 93 377 0 0,-27-20-102 0 0,157-291 72 0 0,-312 423-1909 0 0,108-259 0 0 0,-146 268 211 0 0,-9-4-1 0 0,77-371 0 0 0,0-508 1610 0 0,-125 525-824 0 0,-30 380-477 0 0,-31-195 0 0 0,16 246-142 0 0,-6 1 1 0 0,-6 0 0 0 0,-69-178-1 0 0,55 197 16 0 0,-4 1 0 0 0,-106-169 0 0 0,100 198-10 0 0,-5 4 1 0 0,-1 2-1 0 0,-4 3 0 0 0,-3 2 0 0 0,-3 3 1 0 0,-3 5-1 0 0,-3 2 0 0 0,-2 4 0 0 0,-2 3 0 0 0,-3 3 1 0 0,-141-58-1 0 0,139 74 40 0 0,-3 4 0 0 0,0 5 0 0 0,-2 3 0 0 0,0 4 0 0 0,-109-7 0 0 0,87 18-66 0 0,-1 6 1 0 0,1 4-1 0 0,-214 35 0 0 0,233-18-140 0 0,1 4 0 0 0,0 5 0 0 0,-176 82 0 0 0,186-68-1066 0 0,1 4 0 0 0,2 4-1 0 0,-103 83 1 0 0,79-48-5956 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1032.71">7398 5385 18399 0 0,'-8'3'1408'0'0,"6"-2"-1347"0"0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-3 3 0 0 0,-16 28-212 0 0,9-14 60 0 0,-79 129 266 0 0,59-92 99 0 0,-3-2 0 0 0,-51 64 0 0 0,76-106-267 0 0,-68 77 54 0 0,-130 119-1 0 0,96-118 130 0 0,-127 79-1 0 0,-137 56 643 0 0,124-97-427 0 0,212-108-352 0 0,-154 69 496 0 0,78-37-88 0 0,-23 2-158 0 0,36-16-220 0 0,16-2-55 0 0,-160 42 0 0 0,-8-12 47 0 0,-3-3-74 0 0,-261 64-10 0 0,-229-9-108 0 0,630-108 91 0 0,-1-6-1 0 0,0-5 0 0 0,-1-5 0 0 0,-120-22 1 0 0,-10-26-163 0 0,212 43 108 0 0,-51-26-1 0 0,-2-1 51 0 0,35 15 123 0 0,1-3 0 0 0,-61-38 0 0 0,64 34-103 0 0,9 4-49 0 0,3-2 0 0 0,0-2 0 0 0,2 0 0 0 0,1-3 0 0 0,2-1-1 0 0,-55-69 1 0 0,34 27-81 0 0,4-1-1 0 0,-69-136 0 0 0,75 118 178 0 0,4-4-1 0 0,5 0 0 0 0,-40-168 1 0 0,13-95-301 0 0,59 199-344 0 0,5 152 467 0 0,2-14-571 0 0,-2 14 251 0 0,1-1 0 0 0,-2-12 0 0 0,0 20-54 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 1 0 0,-1-4-1 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2082.08">387 5398 15256 0 0,'-3'0'145'0'0,"2"0"-99"0"0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-2-1 0 0 0,1 0-192 0 0,12 1-882 0 0,75 6 1630 0 0,2 0 129 0 0,-7-5 17 0 0,7 0-176 0 0,155-17-1 0 0,-20-23 149 0 0,-191 37-669 0 0,-27 2-37 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,7-4 0 0 0,-12 6-15 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-13-7 52 0 0,2 4-29 0 0,1 0 0 0 0,-1 1 0 0 0,0 1-1 0 0,0 0 1 0 0,-15 0 0 0 0,11 1-15 0 0,-369 2-25 0 0,331 0-52 0 0,-195 24 134 0 0,9 19-64 0 0,119-19 0 0 0,94-21-60 0 0,1 2 0 0 0,0 1 0 0 0,-32 14 0 0 0,57-20 45 0 0,5-1-18 0 0,6 0 1 0 0,4-2 43 0 0,-1 0 0 0 0,1-1 0 0 0,-1-1 0 0 0,0 0-1 0 0,0-1 1 0 0,0-1 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 0 1 0 0,0-1 0 0 0,-1-1 0 0 0,23-15 0 0 0,-2-5 56 0 0,-1 0 0 0 0,-2-2-1 0 0,31-39 1 0 0,155-221 307 0 0,-198 265-490 0 0,0 0 226 0 0,0-2-38 0 0,39-44 0 0 0,-57 70-67 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,2 2-1 0 0,2 4 70 0 0,0 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,3 14 0 0 0,4 18 225 0 0,54 154 1001 0 0,32 36-675 0 0,1-12-439 0 0,-67-160-437 0 0,60 87-1 0 0,-82-134-816 0 0,0-1 0 0 0,0 0 0 0 0,12 9 0 0 0,-8-8-5638 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3498.42">5794 2852 14064 0 0,'-4'-1'120'0'0,"0"0"1"0"0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,-4-4 1 0 0,4 4-121 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-5-2-1 0 0,-7-1-141 0 0,-7-1-70 0 0,15 5 112 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-9-3 0 0 0,-22-2-453 0 0,8 2 90 0 0,2-1 323 0 0,-49-4 1 0 0,-8 0 482 0 0,-20-9 433 0 0,92 16-617 0 0,-1 1 0 0 0,1 0 0 0 0,-14 2 1 0 0,-13-1 251 0 0,-3 1-78 0 0,1 1 1 0 0,-74 14 0 0 0,23-2-359 0 0,-74 14-18 0 0,126-22 22 0 0,-1-2-1 0 0,-54-3 1 0 0,82-1-17 0 0,-15-1 107 0 0,-50-9 0 0 0,59 5-28 0 0,1 2 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 1 0 0 0,0 1 0 0 0,-33 3 0 0 0,33-1-33 0 0,19-3-55 0 0,-1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,-1 1-1 0 0,-15 12-2493 0 0,8-6-2237 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3946.82">4089 2638 11792 0 0,'0'0'342'0'0,"-1"-1"4"0"0,-1-3-224 0 0,10 11-314 0 0,-6-6 167 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 3 0 0 0,-1-3-8 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 4 0 0 0,-60 190 2512 0 0,55-175-2038 0 0,-3 23 1 0 0,7-36-413 0 0,1-1 0 0 0,1 1 0 0 0,0 0 1 0 0,0-1-1 0 0,2 17 0 0 0,-2-25-112 0 0,0 0-1 0 0,0-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,1-1-1084 0 0,-1 1 1083 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1-835 0 0,0-8-552 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4301.47">4086 2664 6992 0 0,'0'-9'57'0'0,"0"7"-35"0"0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,2-3-1 0 0,-1 3 530 0 0,-2 9-414 0 0,-2 1 81 0 0,0 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,-10 13 1 0 0,0 0 109 0 0,-19 36 26 0 0,12-19 63 0 0,-40 54-1 0 0,52-79 133 0 0,1 0 1 0 0,-11 22-1 0 0,19-36-530 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,2 1 0 0 0,2 0 81 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,6 1 1 0 0,11-1-288 0 0,-11-1-196 0 0,1 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,13 4 0 0 0,-12-1-973 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4903.45">5768 3544 17791 0 0,'-181'-50'1724'0'0,"131"33"-2209"0"0,-60-18-146 0 0,24 7 470 0 0,-12-4 82 0 0,48 19 128 0 0,-166-34 219 0 0,176 41-245 0 0,0 1 0 0 0,-1 2 0 0 0,-59 4-1 0 0,-7 8-58 0 0,-143 30 0 0 0,197-27 12 0 0,0 3 0 0 0,-53 23 0 0 0,91-33 3 0 0,-23 5-1 0 0,10-2-656 0 0,15-11-2658 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5287.29">4112 3239 16184 0 0,'-11'-4'1759'0'0,"10"5"-1764"0"0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 3 0 0 0,3 27-442 0 0,-1-12 208 0 0,3 72 114 0 0,-1-54 127 0 0,-2-1 1 0 0,-6 64-1 0 0,1-75-166 0 0,0 30 0 0 0,4-54-109 0 0,-3-10-4917 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5628.04">4086 3177 11256 0 0,'-16'-2'1133'0'0,"14"3"-1124"0"0,0-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1 3 0 0 0,-19 33 76 0 0,11-18-70 0 0,-8 11 274 0 0,-1-1 0 0 0,-2 0 0 0 0,-1-3 0 0 0,-1 0 0 0 0,-32 28 0 0 0,3-2 1489 0 0,53-52-1778 0 0,-1 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,5 2-45 0 0,-1 1 0 0 0,0-1-1 0 0,10 4 1 0 0,-15-7 42 0 0,217 93-2640 0 0,-187-81 2066 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-12-08T23:00:43.917"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#FFFFFF"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">20 4 18927 0 0,'-10'-4'536'0'0,"5"4"120"0"0,0 2-528 0 0,8 3-2008 0 0,2-1 800 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="355.06">88 82 14656 0 0,'-5'-2'320'0'0,"0"0"72"0"0,1 0 504 0 0,11 2-896 0 0,2-3-4328 0 0,5 1-888 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-12-08T23:00:42.429"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#FFFFFF"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">226 6 11520 0 0,'0'0'673'0'0,"-1"0"-552"0"0,-2-3-122 0 0,2 2-68 0 0,0 1-79 0 0,1 0 135 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0 0 0 0 0,-14 7-220 0 0,13-7 216 0 0,-13 9-141 0 0,0 1 0 0 0,1 0 1 0 0,0 1-1 0 0,1 1 0 0 0,1 0 0 0 0,-22 29 1 0 0,15-10 351 0 0,18-30-178 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 1 0 0 0,0-2 57 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,3 0 0 0 0,21 3 242 0 0,3-2-166 0 0,5 1-151 0 0,58-1 1 0 0,-48-5-927 0 0,-31 1 576 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="858.31">188 53 14368 0 0,'-15'-9'1097'0'0,"14"9"-661"0"0,8 15-1513 0 0,-2 2 758 0 0,-4-13 193 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,5 6 0 0 0,3 4 677 0 0,-10-19-452 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,-3-5 0 0 0,4 8-129 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,-3 0 1 0 0,1 0 17 0 0,0 0 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,1 2 0 0 0,-1-1 0 0 0,1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-5 7 0 0 0,3-4-5 0 0,2 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,0 0-1 0 0,-1 12 1 0 0,3-10 71 0 0,-1 0-1 0 0,1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,9 16 0 0 0,-10-20 23 0 0,0-1 1 0 0,0 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,9 2 0 0 0,-6-3-30 0 0,-1 0 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 1 0 0,12-6 0 0 0,10-6-2112 0 0,-17 7 797 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-12-08T23:00:47.393"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#FFFFFF"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">59 136 12496 0 0,'-11'4'1356'0'0,"9"0"-1562"0"0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1 0 0 0 0,0 7 0 0 0,-1 6-728 0 0,-1-4 682 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,-14 25 677 0 0,20-60 283 0 0,14-100-484 0 0,-15 113-174 0 0,2-12 387 0 0,0-25 740 0 0,-3 58-921 0 0,0 8 62 0 0,0 27 367 0 0,1-43-644 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,4 7 0 0 0,-5-10-37 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 1 0 0,-1-1-4 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-3 0 0 0,2-3-3 0 0,0 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,3-8 1 0 0,-3 1 159 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,-7-25 1 0 0,10 37-133 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,-2 11 288 0 0,3 16-356 0 0,8 24-525 0 0,0-17-3894 0 0,-1-3-1041 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-12-08T23:02:40.228"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">136 838 8208 0 0,'0'0'234'0'0,"-1"0"6"0"0,-4 0-558 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,0 0-1 0 0,-7 5 0 0 0,-8 5-101 0 0,15-10 633 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 9 0 0 0,2-11-129 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,1 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0-1-1 0 0,3 2 1 0 0,0-1-19 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 1-1 0 0,0-2 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,9-7 1 0 0,-6 3 6 0 0,-1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-2 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,7-15-1 0 0,-8 15-56 0 0,-1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-2-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-3-10-1 0 0,2 13 29 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-5-2 0 0 0,3 2 6 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,-12 4 1 0 0,15-2-168 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-3 4 1 0 0,-10 11-3641 0 0,11-6-101 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="461.41">361 813 9072 0 0,'0'0'22'0'0,"0"0"0"0"0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,4 4-57 0 0,3 6-750 0 0,0 1 0 0 0,8 18 0 0 0,-13-26 574 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-2 6 1 0 0,0-1-487 0 0,1-3 801 0 0,-1 1-1 0 0,0-1 0 0 0,-4 13 2067 0 0,5-23-2014 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-3-5 1 0 0,-1-5 6 0 0,3 9-31 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,3-8 0 0 0,0 3-24 0 0,0 1 0 0 0,0 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,15-14 0 0 0,-16 17-400 0 0,22-20 574 0 0,-25 25-500 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,3 0 0 0 0,0 2-2637 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="891.2">755 808 9760 0 0,'0'0'908'0'0,"-16"2"-5600"0"0,9-1 3819 0 0,0 1 0 0 0,0 0 1 0 0,-7 3-1 0 0,8-3 1579 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-6 5 1 0 0,11-8-378 0 0,-1-1-207 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 2 0 0 0,2-2-105 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,3-1 0 0 0,-1-1-94 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,4-6 1 0 0,-7 9 82 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 1 0 0 0,9 11 105 0 0,-8-9-129 0 0,15 37-834 0 0,-14-32 437 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1241.35">955 744 7616 0 0,'0'0'472'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1641.23">855 740 5248 0 0,'-14'4'325'0'0,"12"-4"-298"0"0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-2 1-1 0 0,0 3 139 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 10 0 0 0,2-11-134 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,2 4 0 0 0,-1-4 47 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,6 3 0 0 0,-7-5-43 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,2 0-1 0 0,-1 0-24 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0-5 1 0 0,0-21 125 0 0,-1 29-137 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,12 12 38 0 0,-9-1 109 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,-1 1-1 0 0,-1 16 1 0 0,1-8 176 0 0,4 24 1 0 0,-2-27-353 0 0,4 20 420 0 0,3-13-3754 0 0,-7-20-316 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2073.66">1144 786 9184 0 0,'-8'-7'704'0'0,"5"5"-644"0"0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-3-4 0 0 0,4 5-57 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,-4-1 1 0 0,5 2-43 0 0,-1 1 1 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,-2 3-4 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,0 1 0 0 0,-4 8 0 0 0,6-9 223 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 10 0 0 0,1-13-98 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,3 3 0 0 0,-3-4-73 0 0,1 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,2-1 1 0 0,2-1-55 0 0,1-1 1 0 0,-1 0 0 0 0,0 0-1 0 0,7-8 1 0 0,-7 6-5 0 0,1 0 1 0 0,-1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,2-12-1 0 0,-5 19 114 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,4 5 343 0 0,1 12-1175 0 0,-3-9 342 0 0,-1 1 1 0 0,0 0 0 0 0,-1 0 0 0 0,-1 9 0 0 0,1 3-1303 0 0,0-9-2071 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2456.57">1273 701 8840 0 0,'0'0'658'0'0,"15"3"-371"0"0,-13-2-255 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0 3 0 0 0,1 4-1 0 0,-1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-2 12 0 0 0,0-1 28 0 0,3-16-71 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,-3 7 1383 0 0,5-21-443 0 0,-1 4-725 0 0,1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,3-11 1 0 0,1-2-101 0 0,-4 13-102 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,5-5 0 0 0,-8 9-4 0 0,1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,1 1 0 0 0,-2-1-4 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 2 0 0 0,2 5-25 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,1 13 0 0 0,0 64-1120 0 0,4-67-1454 0 0,-6-17 1262 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2809.84">1493 666 9968 0 0,'0'0'584'0'0,"16"2"-326"0"0,-14-1-224 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 2 1 0 0,3 6 45 0 0,-1 0 0 0 0,4 13 1 0 0,-8-21-49 0 0,3 8-233 0 0,0-1 1 0 0,-1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,-2 17 0 0 0,1-13-1153 0 0,-2-1 0 0 0,-7 22 1 0 0,10-34 1292 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 22 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-2 0 0 0,-2-4-1135 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3207.23">1525 712 8928 0 0,'19'4'640'0'0,"-9"-3"-599"0"0,0 0 1 0 0,1-1-1 0 0,-1 0 1 0 0,0-1-1 0 0,13-2 1 0 0,52-15 376 0 0,-7 1-221 0 0,21 1 459 0 0,-99 18-182 0 0,1 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,0 1 0 0 0,0-1-1 0 0,-10 8 1 0 0,-10 5-128 0 0,23-13-297 0 0,0-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0-1 1 0 0,1 1-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,-5 11 0 0 0,6-12-193 0 0,1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,4 8-1 0 0,-4-11-109 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,4 0 1 0 0,10-2-1413 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3621.5">1966 637 12240 0 0,'-1'0'37'0'0,"0"-1"0"0"0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-2 2 0 0 0,0-1-52 0 0,0 1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,-1 4-1 0 0,-2 4-1078 0 0,1 0-1 0 0,-6 19 1 0 0,8-23 119 0 0,-8 27-2232 0 0,13-38 6144 0 0,-1 0-2821 0 0,41-111 3614 0 0,-41 104-3307 0 0,0 2 484 0 0,0 20-405 0 0,3 50-1207 0 0,-3-29-1362 0 0,11 55 0 0 0,-11-76-1902 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3622.5">2168 0 11024 0 0,'0'0'248'0'0,"-8"15"613"0"0,7 1-834 0 0,0 1 1 0 0,1 0-1 0 0,4 27 0 0 0,0 15-83 0 0,-1 214-993 0 0,1-156-2328 0 0,-4-71 33 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4037.07">1916 518 10568 0 0,'0'0'1160'0'0,"5"0"-1160"0"0,0 0 0 0 0,6 5 0 0 0,4-3 64 0 0,4 0-64 0 0,5 1 64 0 0,-1-1-288 0 0,4 0-48 0 0,1-2-16 0 0,-1 3 0 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-12-08T23:03:31.959"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">12 181 7256 0 0,'-6'-56'2452'0'0,"6"50"-2419"0"0,0-5 2195 0 0,3 19-1547 0 0,11 57-872 0 0,-5-28 172 0 0,4 45 0 0 0,-12-45 40 0 0,-1-36 417 0 0,-11-16-350 0 0,3-11-386 0 0,1 0 0 0 0,1 0 0 0 0,-4-50 0 0 0,8 59 148 0 0,1-1 0 0 0,0 0 0 0 0,2 1 0 0 0,4-35 0 0 0,-4 49 155 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,3-4 1 0 0,-3 5 25 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 1 0 0 0,2-1 0 0 0,6 2 60 0 0,-1 0 1 0 0,1 1-1 0 0,13 6 1 0 0,16 4-69 0 0,-36-12-21 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,3 2 0 0 0,-6-3 44 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 1 0 0,-3 2-1 0 0,4-4-38 0 0,-17 18 129 0 0,11-13-148 0 0,0 1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0-1 0 0,-6 13 1 0 0,0 5-1083 0 0,9-13-44 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="584.72">337 149 11024 0 0,'0'0'1189'0'0,"19"-3"-1634"0"0,-16 4 425 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,3 3 0 0 0,1 2 69 0 0,-1 0 1 0 0,8 12 0 0 0,5 6-278 0 0,-3-2 405 0 0,-15-20-113 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 0 0 0 0,4 2 0 0 0,-4-2-44 0 0,0 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,4-4 0 0 0,-3 2-88 0 0,0 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-7 1251 0 0,12 16-575 0 0,-7 1-598 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1-1 0 0,7 11 1 0 0,15 20-279 0 0,4-2-1249 0 0,-24-28-2940 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="922.89">870 30 16416 0 0,'0'0'1249'0'0,"-5"2"-715"0"0,5-2-533 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,2 10-37 0 0,-1 1 0 0 0,2 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,0-1 0 0 0,7 17 0 0 0,4 10-106 0 0,-11-29 48 0 0,44 144-2190 0 0,-40-120-428 0 0,4 36-1 0 0,-10-42 924 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink7.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-12-08T23:06:52.732"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">3491 534 16783 0 0,'-35'-29'642'0'0,"1"-2"0"0"0,-40-47-1 0 0,51 53-718 0 0,-8-8-320 0 0,-1 1 0 0 0,-2 1-1 0 0,-72-50 1 0 0,70 59 282 0 0,-1 2-1 0 0,-1 1 1 0 0,-56-19-1 0 0,37 20-59 0 0,-108-20 0 0 0,28 20-212 0 0,-184 0 0 0 0,89 16 538 0 0,0 10 0 0 0,-287 46 0 0 0,441-39-105 0 0,0 2 0 0 0,2 5 0 0 0,0 2 0 0 0,2 4 0 0 0,-87 45 0 0 0,100-40-193 0 0,2 2 0 0 0,1 3 0 0 0,2 3 0 0 0,2 1 1 0 0,2 4-1 0 0,-60 66 0 0 0,80-76-375 0 0,3 2-1 0 0,1 1 1 0 0,1 1-1 0 0,-35 74 1 0 0,47-81-79 0 0,2 0-1 0 0,1 1 1 0 0,1 1 0 0 0,2 0-1 0 0,2 0 1 0 0,-6 68 0 0 0,13-84 238 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,2 0 0 0 0,0-1 0 0 0,2 0 0 0 0,0 1 0 0 0,0-2 0 0 0,15 31 0 0 0,-12-33 198 0 0,1 0 0 0 0,0-1-1 0 0,1 0 1 0 0,0 0 0 0 0,2-1 0 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,27 16 1 0 0,-14-12 287 0 0,1-2 0 0 0,0 0 0 0 0,1-2 0 0 0,0-1 0 0 0,42 9-1 0 0,-10-8 586 0 0,101 8-1 0 0,-15-14 404 0 0,174-15 0 0 0,144-42-173 0 0,235-68 412 0 0,-16-69-779 0 0,-314 32-141 0 0,-289 120-231 0 0,-9 3 525 0 0,-2-2 0 0 0,-1-3 1 0 0,84-65-1 0 0,-130 86-385 0 0,0-1 0 0 0,-1 0-1 0 0,19-25 1 0 0,-32 34-215 0 0,-1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,4-21 0 0 0,-7 24-66 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,-8-12 0 0 0,0 3 35 0 0,-1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-26-18-1 0 0,5 8-209 0 0,-1 1-1 0 0,-2 2 1 0 0,0 1-1 0 0,-50-17 1 0 0,-168-43-600 0 0,115 47 676 0 0,-2 6 0 0 0,0 6-1 0 0,-1 7 1 0 0,-1 5 0 0 0,0 8 0 0 0,0 5 0 0 0,-203 33 0 0 0,223-15-1081 0 0,-202 65 1 0 0,37 23-3833 0 0,148-46 1123 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink8.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-12-08T23:10:47.212"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">3 421 6296 0 0,'-2'-3'2349'0'0,"2"4"-2299"0"0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,1 0 0 0 0,8 9 371 0 0,-6-3-359 0 0,0 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,0 0 0 0 0,2 11-1 0 0,1 16 56 0 0,-3-31-106 0 0,-1-4 117 0 0,1 0 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,4-2 0 0 0,8-1-71 0 0,-8 1-31 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,1-2 1 0 0,-1 1-1 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,7-7 1 0 0,49-66 26 0 0,-41 50-44 0 0,3-1 230 0 0,2 0 1 0 0,42-33 0 0 0,-58 52-174 0 0,76-61 527 0 0,20-19-353 0 0,-37 34-129 0 0,-25 22-732 0 0,-17 12-2624 0 0,1 3-1148 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink9.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-12-08T23:11:37.725"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">386 669 10680 0 0,'-7'-6'138'0'0,"-1"-1"-1"0"0,1 1 1 0 0,0-1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-8-15-1 0 0,11 20-137 0 0,2 2 170 0 0,-6 10-484 0 0,-9 140 308 0 0,-23 199 60 0 0,9-16-17 0 0,17 433 0 0 0,61-83-500 0 0,4 106-92 0 0,-68 144 567 0 0,-6-628 383 0 0,-11 198 506 0 0,22-2 136 0 0,33 21-382 0 0,-21-482-1289 0 0,-2-30 300 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1576.61">202 553 10384 0 0,'-6'-10'257'0'0,"5"10"-247"0"0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,12-9-79 0 0,1 0-1 0 0,0 1 1 0 0,1 1 0 0 0,0 2-1 0 0,32-12 1 0 0,-25 10 17 0 0,88-30 46 0 0,2 5 1 0 0,165-26-1 0 0,242 9 10 0 0,-111 31-4 0 0,-81-4 300 0 0,-90 4 16 0 0,346-30 671 0 0,-406 31-974 0 0,212-26-13 0 0,43-3 0 0 0,386 5 210 0 0,-809 42-208 0 0,158 3 32 0 0,-127-1-28 0 0,-1 3 0 0 0,45 10 0 0 0,-67-10-6 0 0,1 1 0 0 0,26 11 0 0 0,-36-13 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,10 10 0 0 0,-4-2 0 0 0,-8-9 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,5 7 0 0 0,-4-2 0 0 0,7 11 0 0 0,-2 1 0 0 0,0 1 0 0 0,11 40 0 0 0,27 210 216 0 0,-40-196-96 0 0,-4 123 0 0 0,-39 161 307 0 0,-24-3-12 0 0,1-10-321 0 0,-40 663-773 0 0,60-450 366 0 0,24-329 322 0 0,-25 588 228 0 0,68-53 1629 0 0,32-238-1642 0 0,-54-478-224 0 0,28 215 0 0 0,1 46 1757 0 0,-29-259-324 0 0,-6-53-1406 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,-1 0-23 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 1-1 0 0,-6-2 13 0 0,1 1 0 0 0,-1-1 0 0 0,-13-4 0 0 0,-31-10-225 0 0,2-2 1 0 0,0-3-1 0 0,-71-36 0 0 0,74 35 172 0 0,-2 2 0 0 0,-82-19-1 0 0,95 28 22 0 0,-45-11-39 0 0,-1 3 0 0 0,-104-8 0 0 0,122 20 129 0 0,7 0 101 0 0,-119 3-1 0 0,96 10-63 0 0,-226 12 164 0 0,-115 25-274 0 0,200-17 0 0 0,164-21-2 0 0,-105 14 263 0 0,-54 9 497 0 0,-2 0-375 0 0,-1 0-88 0 0,88-13-110 0 0,-453 61 378 0 0,369-51-261 0 0,-252-1 0 0 0,281-28-650 0 0,-118 2 855 0 0,183 4-2141 0 0,114-4-3397 0 0,2-1-1621 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14791.72">613 1081 6880 0 0,'-1'-10'864'0'0,"1"5"1825"0"0,1 13-1732 0 0,0 0-880 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,-2 16-1 0 0,0 0 16 0 0,-8 51 878 0 0,6-49-373 0 0,-5 19 779 0 0,11-70-1661 0 0,8-42 1 0 0,-3 29-135 0 0,-4 18 259 0 0,2-1 0 0 0,0 1 0 0 0,1 1 0 0 0,1-1 0 0 0,1 1 1 0 0,1 0-1 0 0,11-21 0 0 0,-15 35 137 0 0,-1 0 1 0 0,1-1-1 0 0,7-7 0 0 0,-9 11 12 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,6 0 1 0 0,3-1-39 0 0,-10 3 47 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 0 0 0,4 1 24 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 2 0 0 0,-1-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-2 9 1 0 0,0-8 77 0 0,0-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,-1-2-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,-10 4 1 0 0,-11 0-47 0 0,20-4-231 0 0,-1 0-973 0 0,8-5 999 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,-1-6-3812 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15291.61">953 1147 9616 0 0,'0'-3'90'0'0,"1"0"0"0"0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,2-3 0 0 0,-2 4-33 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,2 0 0 0 0,-3 1-23 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,8 24-77 0 0,-7-13 72 0 0,-1 1 0 0 0,-1-1 1 0 0,-1 13-1 0 0,0 7-1774 0 0,1-25-1974 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15670.65">1071 1286 11312 0 0,'16'-9'1133'0'0,"-1"6"-1024"0"0,-15 2-97 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 24 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1-1 0 0 0,2 0 1 0 0,-2 1-118 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,1 0-1 0 0,0 1 1 0 0,-1-3-147 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0-2-1 0 0,0-2 130 0 0,-1 3-226 0 0,1 1 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-1-4 0 0 0,0 2 158 0 0,-8-25-1121 0 0,9 27 1310 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,-1-2 0 0 0,-13-8 808 0 0,14 9-609 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,-3-1 0 0 0,-2 1 167 0 0,7 1-256 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,-2-1 0 0 0,3 1 53 0 0,22-4-1016 0 0,-18 5 833 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,2-1 0 0 0,-3 1-93 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,2-1 0 0 0,5-1-2414 0 0,-2-2-830 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16329.22">1352 1150 12624 0 0,'0'0'740'0'0,"0"5"-582"0"0,-17 228-2512 0 0,16-229 2258 0 0,1 2 76 0 0,-3 12 737 0 0,3-18-710 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-3-13 193 0 0,1-12-223 0 0,0-2 0 0 0,3-37 0 0 0,0 12 4 0 0,-1 42 19 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 2 0 0 0,-1-1 0 0 0,2-1 0 0 0,-1 1 0 0 0,7-16 0 0 0,0 8 6 0 0,-7 12 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,4-3 0 0 0,-6 7-5 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,2 0 0 0 0,0 1 21 0 0,-1-1-19 0 0,-1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,4 1 0 0 0,-5-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 1 48 0 0,1 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,2 9 0 0 0,-4-11 7 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-3 4-1 0 0,-7 16 216 0 0,8-18-244 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-3 5 1 0 0,-8 4 17 0 0,9-9-146 0 0,0 1 1 0 0,0 0 0 0 0,-5 6-1 0 0,10-10-270 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16688.04">1541 1177 7456 0 0,'0'0'166'0'0,"4"-2"409"0"0,-4 1-558 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,-5 13 204 0 0,3-9-110 0 0,-5 25 338 0 0,-8-38 616 0 0,14 10-1006 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 2 1 0 0,-8 10 2323 0 0,22-13-1742 0 0,44-31-491 0 0,-38 23-295 0 0,-17 8 128 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,1-2 0 0 0,-2 4 18 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,3 6 6 0 0,-1 10 82 0 0,-5 12 643 0 0,3-23-547 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,0 8 0 0 0,2-6-474 0 0,3-9-1932 0 0,-2 0-751 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17046.76">1723 996 8208 0 0,'0'0'234'0'0,"10"-13"108"0"0,-7 10-161 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,5-3 0 0 0,0-2 12 0 0,-4 4-34 0 0,-3 4-142 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 2 176 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 3 1 0 0,2 6 536 0 0,1 26-1 0 0,-2-21-434 0 0,1 8 39 0 0,1-2 0 0 0,14 45 1 0 0,-17-65-362 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,4 3 1 0 0,-7-5-64 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,2-5-4771 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17385.34">1735 1145 9072 0 0,'0'0'681'0'0,"14"7"70"0"0,-13-7-675 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 2-55 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 24 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,3 0 1 0 0,3-1 85 0 0,0 1 0 0 0,0-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,6-3 1 0 0,-2 0-122 0 0,1 1 1 0 0,-1 0 0 0 0,22-5 0 0 0,-20 7-132 0 0,-11 2 67 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,2-2 0 0 0,9-9-4747 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17742.75">2155 1098 13216 0 0,'0'0'298'0'0,"-1"-4"1140"0"0,-14 31-1630 0 0,14-26 166 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,-8 3-206 0 0,7-2 122 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,-3 0 0 0 0,4 0 120 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-3 3 0 0 0,4-4 55 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 2 1 0 0,2-1 58 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,1 2 1 0 0,5 4-350 0 0,-6-4 228 0 0,1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,5 1 1 0 0,6 1-172 0 0,-12-2 27 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,3-1 1 0 0,4-4-4837 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18111.21">2291 791 8208 0 0,'0'0'474'0'0,"-13"15"1946"0"0,11 1-1371 0 0,1 0-1 0 0,0 0 1 0 0,2 26-1 0 0,0-5-318 0 0,2 17-404 0 0,3 1 0 0 0,19 83 0 0 0,-22-124-303 0 0,9 21-11 0 0,-6-18-1 0 0,-6-17 11 0 0,0 1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 0 0 0 0,0-1-4 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,1-4-1 0 0,25-53 53 0 0,7-15-276 0 0,-33 72 216 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,9 15-54 0 0,-2 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,-1-2 0 0 0,5 31 0 0 0,-10-44-1332 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19108.58">3364 804 4464 0 0,'0'0'329'0'0,"-1"0"-223"0"0,-2-1-74 0 0,2 1 100 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2-117 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-13 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1-1 0 0 0,1 2 0 0 0,3 17 89 0 0,0 0-1 0 0,-1 0 1 0 0,-1 1 0 0 0,-1-1 0 0 0,0 32 0 0 0,0-14-64 0 0,-9 218 112 0 0,6-242-137 0 0,-9 56-179 0 0,9-57 68 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19691.75">3341 759 9072 0 0,'0'0'200'0'0,"19"5"536"0"0,33-5-888 0 0,-40 0 138 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,21-6 0 0 0,15-2 3 0 0,72-12-768 0 0,3-1 35 0 0,-32 11 1392 0 0,-22 6 640 0 0,-1-4 0 0 0,98-24 0 0 0,-62 11-1214 0 0,148-13 0 0 0,-198 28-313 0 0,-1-1 1 0 0,57-20-1 0 0,-84 23 273 0 0,0 0 0 0 0,0 2 0 0 0,0 1 0 0 0,36 1 0 0 0,31-2-1 0 0,-32 3-3595 0 0,-52 0 2324 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20553.74">3412 1381 7688 0 0,'1'0'31'0'0,"0"0"0"0"0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,2 0 0 0 0,15-2 264 0 0,-8 3-178 0 0,0 0 1 0 0,17-2-1 0 0,-6-1 99 0 0,6 2 264 0 0,-15 1-396 0 0,0-1 0 0 0,0 0 0 0 0,17-4 0 0 0,200-37 404 0 0,-154 32-408 0 0,-44 6-45 0 0,-13 2 43 0 0,25-5 1 0 0,15-7 128 0 0,-26 8 153 0 0,33-13 1 0 0,-42 12-102 0 0,30-6 0 0 0,4 0 63 0 0,22-7-6 0 0,23-5 60 0 0,-89 21-298 0 0,0 1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,18 2 1 0 0,-14-1 0 0 0,1 0 0 0 0,20-4 0 0 0,-20 2-62 0 0,38-1 0 0 0,-35 4-2 0 0,25-5 0 0 0,25-1 27 0 0,-7 1 110 0 0,-22 3-95 0 0,-30 2-58 0 0,0 0 0 0 0,15-3 0 0 0,-26 3-1 0 0,5-2 10 0 0,1 1 0 0 0,-1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,7 2 1 0 0,-13-2 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 13 0 0,-1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,1 0 0 0 0,10 5 298 0 0,-11-4-235 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,2 1-1 0 0,-4-2-26 0 0,0 1-69 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1-2-75 0 0,0 4 77 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 1-1 0 0,2 7-211 0 0,0 0-67 0 0,-3-8 276 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,2-15-1076 0 0,-2 11 702 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21505.33">5070 585 3712 0 0,'0'0'280'0'0,"-5"-5"-176"0"0,2-7 8274 0 0,6 16-9398 0 0,-1 6 1421 0 0,0 1-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,-2 18 1 0 0,0 26 298 0 0,0 238-461 0 0,1-186 16 0 0,1-58 322 0 0,1-22-430 0 0,0-22-328 0 0,0-17 114 0 0,-9-131 300 0 0,0-204-4382 0 0,8 340 4278 0 0,-1 4-103 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,2-3 0 0 0,-2 5-115 0 0,9 6-2326 0 0,-8-1 2466 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 2 0 0 0,-1-1 0 0 0,2 8 0 0 0,3 34 1484 0 0,0 10-839 0 0,3 46-555 0 0,-2-4-136 0 0,-6-85 2 0 0,1 0 58 0 0,7 23-1 0 0,0 5-1082 0 0,-8-29 541 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26157.98">597 2232 9168 0 0,'0'0'1469'0'0,"5"13"-1325"0"0,3 32-188 0 0,5 68 0 0 0,-10 13-128 0 0,-4-105 163 0 0,-1 6 225 0 0,2-26 448 0 0,-5-18 96 0 0,-2-20-1353 0 0,1-1 0 0 0,2-1 0 0 0,2-38 0 0 0,8 13-910 0 0,-3 38 947 0 0,0 12 257 0 0,-2 11 279 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1-1 0 0 0,0-3 0 0 0,0 6 716 0 0,1 1-632 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,2 5-102 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,-4 12 0 0 0,2-10 39 0 0,0 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1-1 0 0 0,-11 11-1 0 0,10-11-572 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27049.62">756 2426 11808 0 0,'0'0'1180'0'0,"14"12"-786"0"0,-13-11-440 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 1 0 0,0 7-927 0 0,0-8 327 0 0,1-1 679 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,-1-10 77 0 0,2 10-97 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 1 16 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1-1 0 0,7-4 692 0 0,-7 4-722 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 3 0 0 0,14 18-20 0 0,-13-15 89 0 0,3 3 81 0 0,0 0 1 0 0,-1 1 0 0 0,0 0-1 0 0,7 21 1 0 0,-12-25-94 0 0,0-6-171 0 0,-3-11-432 0 0,-1 2 525 0 0,0 0-1 0 0,-9-14 0 0 0,11 20 18 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-5-3 0 0 0,7 5-114 0 0,-9-6-1058 0 0,8 35 2090 0 0,2-26-829 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,2 4 1 0 0,0-2-86 0 0,-2-5 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1-2-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,-1-5 0 0 0,1 1-11 0 0,0 3-5 0 0,-1 1-1 0 0,0-1 0 0 0,1 0 1 0 0,-4-7-1 0 0,-1-11 1215 0 0,5 23-1276 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 3 0 0 0,-1 6 53 0 0,1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,1 0 0 0 0,5 16 0 0 0,1 2-183 0 0,-2-1-668 0 0,-6-26 327 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28115.89">850 2344 8784 0 0,'0'0'658'0'0,"0"0"-447"0"0,0-4 1065 0 0,0 3-1203 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0-26 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 1 0 0,-3 1-1 0 0,0 1-120 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 3 0 0 0,-4 5 65 0 0,6-9 35 0 0,1 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 1 1 0 0,-4 13 261 0 0,4-13-288 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 3 0 0 0,2 9 38 0 0,-3-14-23 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 1 0 0,1 3-1 0 0,1-1 28 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 0-1 0 0,4-1 1 0 0,10-3 237 0 0,-13 3-169 0 0,-1 1 1 0 0,1-1-1 0 0,11-5 1 0 0,6-6-125 0 0,-1 0 0 0 0,43-31 0 0 0,-58 37 24 0 0,1 0 1 0 0,-1-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1-1-1 0 0,5-9 1 0 0,-8 13 8 0 0,0 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-7-1 0 0,-1 13 103 0 0,8 18 18 0 0,-1 1-59 0 0,0 1 0 0 0,-2-2 0 0 0,7 38 0 0 0,-1 62 115 0 0,-9-98-202 0 0,9 49-2663 0 0,-9-56 636 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29518.65">481 3073 9416 0 0,'0'0'706'0'0,"-1"-1"-482"0"0,0-2-157 0 0,0 2 357 0 0,4 12 291 0 0,2 18-449 0 0,2 53 0 0 0,-5-58-150 0 0,16 144 556 0 0,-17-160-614 0 0,0-1 125 0 0,0 0 1 0 0,0 1-1 0 0,5 9 1 0 0,-6-17 296 0 0,1-2-446 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-4 0 0 0,-1 7-30 0 0,2-33-180 0 0,-2-1-1 0 0,-5-41 0 0 0,2 39-305 0 0,2-57 0 0 0,2 84 466 0 0,1 0-1 0 0,4-16 1 0 0,1 0-11 0 0,-7 24 29 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,2-2 1 0 0,-3 3 5 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,2 1 5 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 2 1 0 0,0-1-1 0 0,3 5 0 0 0,0 4-9 0 0,1-1 0 0 0,-2 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 15 0 0 0,-2-13 231 0 0,0-1 1 0 0,-1 1 0 0 0,-1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,-1 0-1 0 0,-1 1 1 0 0,0 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,-10 23 0 0 0,9-28-125 0 0,0 1 1 0 0,0-2 0 0 0,-1 1 0 0 0,-7 9 0 0 0,10-15-151 0 0,0 0 0 0 0,0 1 0 0 0,0-2 0 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-4 2 0 0 0,-3-3-4770 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="30477.69">995 3112 10680 0 0,'0'0'241'0'0,"-6"-18"734"0"0,6 17-938 0 0,1 1 1 0 0,-1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,0-1-60 0 0,0 1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-2 1 0 0 0,-3 1-172 0 0,1 1-1 0 0,-1 0 1 0 0,-8 5 0 0 0,-8 11 284 0 0,20-17-62 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-2 3-1 0 0,-6 29 652 0 0,8-29-597 0 0,1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,3 6-1 0 0,-1-2 4 0 0,1-2 0 0 0,0 0-1 0 0,1 1 1 0 0,0-1 0 0 0,8 10-1 0 0,-6-11 22 0 0,-1 0-1 0 0,2 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 0 0 0 0,0-1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0-1 0 0 0,19-1 1 0 0,-24-1-63 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,2-9 0 0 0,-3 8-5 0 0,0 0 0 0 0,0-1 0 0 0,-1 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 2 0 0 0,0-2 0 0 0,-4-7 0 0 0,2 9 14 0 0,-1-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,-13-6 0 0 0,-5-1-49 0 0,-44-17-1 0 0,41 19-517 0 0,13 5-1041 0 0,2 2-4458 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="31680.74">3362 2129 9936 0 0,'0'0'746'0'0,"5"9"-380"0"0,-4 0-344 0 0,0-1-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1 10 0 0 0,0 6 11 0 0,-2 75 614 0 0,0-47-615 0 0,6 71-1 0 0,-1-80 33 0 0,-2-33-260 0 0,0 0 0 0 0,1 1-1 0 0,0 0 1 0 0,1-1 0 0 0,5 21-1 0 0,-4-26-2480 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="32560.07">3236 2121 13216 0 0,'0'0'1326'0'0,"12"-7"-1204"0"0,-5 3-89 0 0,1 0 1 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,16-3 0 0 0,-2 1-47 0 0,171-38 889 0 0,117-27-843 0 0,-193 41 284 0 0,190-53-247 0 0,-217 52-74 0 0,150-28 0 0 0,-214 54 28 0 0,-1 0 0 0 0,1 2 0 0 0,49 4 0 0 0,-55-1-59 0 0,0 1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 2 0 0 0,31 13 1 0 0,-40-16 16 0 0,0 3 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 1-1 0 0,0 1 1 0 0,12 13 0 0 0,-17-16 48 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 2 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 11 1 0 0,-8 127 125 0 0,14 8-610 0 0,-7-120 350 0 0,0-15 102 0 0,-3 23 1 0 0,1 32 49 0 0,2-42 110 0 0,-3-17-229 0 0,2-12 196 0 0,-25 8 201 0 0,14-7-359 0 0,0-1 0 0 0,-12-1 0 0 0,-13 1-101 0 0,-17 1-34 0 0,-74-7-1 0 0,80 2 189 0 0,-98 1-201 0 0,-166 7 134 0 0,63-2 591 0 0,186-1-679 0 0,0 3 0 0 0,1 3 0 0 0,-1 2-1 0 0,2 4 1 0 0,0 1 0 0 0,0 3-1 0 0,-67 31 1 0 0,72-24-4439 0 0,29-13-43 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="33217.74">3382 2916 8840 0 0,'0'0'658'0'0,"11"16"-4"0"0,9 11-42 0 0,-16-22-651 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,2 7-1 0 0,0 3 29 0 0,-1 1-1 0 0,-1-1 1 0 0,3 28 0 0 0,-4 51-1 0 0,-1-25 11 0 0,0-19-70 0 0,3 35-182 0 0,-7-30-970 0 0,3-54 934 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="34107.6">3284 2958 14600 0 0,'0'0'1100'0'0,"8"1"-600"0"0,39 0-1366 0 0,-3 0 556 0 0,80-8 0 0 0,172-50 1543 0 0,-94 15-996 0 0,-83 16-271 0 0,-41 7-8 0 0,-30 8-4 0 0,224-38 695 0 0,-253 46-582 0 0,0 2-1 0 0,-1 0 0 0 0,1 2 1 0 0,0 0-1 0 0,0 1 0 0 0,22 4 0 0 0,-24-1-220 0 0,22 8 0 0 0,-34-10 108 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,4 5 1 0 0,-7-8 47 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,0 2-1 0 0,-1 2 138 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,-3 3-1 0 0,-2 5 413 0 0,0 2-582 0 0,1 1-1 0 0,1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,1 2 1 0 0,0-1-1 0 0,1 1 0 0 0,1 0 1 0 0,1 0-1 0 0,2 23 0 0 0,2 21 34 0 0,5 65-78 0 0,-6-104 75 0 0,-1-2 0 0 0,6 28 0 0 0,-3-27 89 0 0,6 19 493 0 0,-2-18-480 0 0,12 34-72 0 0,-20-53-94 0 0,-1-1-3 0 0,-1-2 62 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 1 1 0 0,1-2-1 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 1 0 0,-2-2 6 0 0,-37-18 242 0 0,-76-29 0 0 0,91 41-299 0 0,0 2 0 0 0,-1 1 0 0 0,1 1 0 0 0,-45-3-1 0 0,-89 3-45 0 0,-89-6 276 0 0,186 7-66 0 0,-1 3-1 0 0,1 3 1 0 0,0 2-1 0 0,-98 20 1 0 0,113-14-196 0 0,17-4-328 0 0,-1 0 1 0 0,-54 22-1 0 0,6 2-3284 0 0,49-19 2326 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="40990.14">1412 2807 9408 0 0,'0'0'541'0'0,"19"3"-50"0"0,-17-2-509 0 0,1 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,3 2 0 0 0,12 9-71 0 0,-16-12 119 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,1-2-1 0 0,2 0 134 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,3-4-1 0 0,-5 5-132 0 0,28-25 773 0 0,-28 26-755 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,2 2 0 0 0,2 1-16 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,5 7 0 0 0,-6-7-11 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,6 4-1 0 0,-6-5-18 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,3 0 0 0 0,28-14 43 0 0,-27 12-44 0 0,7-4-48 0 0,23-18 0 0 0,9-4-30 0 0,-37 24 91 0 0,-3 2 50 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 1 0 0,0 2-1 0 0,0-1 0 0 0,0 0 0 0 0,9 0 1 0 0,7-1 602 0 0,-18 3-668 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,4-2 0 0 0,5-1 0 0 0,32-10 0 0 0,-27 8 0 0 0,2 0 0 0 0,30-4 0 0 0,-40 9 31 0 0,5-1-56 0 0,0 0 1 0 0,1 1 0 0 0,-1 1 0 0 0,1 0 0 0 0,28 5 0 0 0,-38-3 2 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,5 4 0 0 0,8 8-4900 0 0,-13-10 309 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="42304.8">1197 3771 9960 0 0,'0'0'1656'0'0,"5"15"-1618"0"0,2 33 373 0 0,-6-38-297 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0-1 0 0 0,8 18 0 0 0,-10-26-90 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,1 0-1 0 0,4-3 152 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,5-6 0 0 0,-7 6-197 0 0,2-2 53 0 0,-1 0 1 0 0,9-14-1 0 0,-9 13-44 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,13-12 1 0 0,-17 17 15 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,4 1 0 0 0,9 5 19 0 0,24 15 193 0 0,-35-20-196 0 0,0 0 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,6-2-1 0 0,-3 0-152 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,7-6 1 0 0,-9 7 139 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 1 0 0,1 1-1 0 0,7-4 0 0 0,-9 5 77 0 0,-1 2 3 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-2 0 0 0,1 2 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,2 3 1 0 0,-1-2-92 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,6 5 1 0 0,-6-6-28 0 0,0 1 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,5-3 0 0 0,-2 1-121 0 0,-1 0 1 0 0,1-1-1 0 0,0 0 1 0 0,9-7-1 0 0,-9 6 79 0 0,0 0 0 0 0,0 1-1 0 0,11-5 1 0 0,-13 7 110 0 0,-1 0-1 0 0,1 0 1 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,6 4-1 0 0,2 3-153 0 0,0 0 0 0 0,0 0 0 0 0,18 22 1 0 0,-17-17-108 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="46068.58">6290 2109 6968 0 0,'-79'7'608'0'0,"32"-2"-1475"0"0,-86-4-1532 0 0,64-2 4207 0 0,37 1-1666 0 0,-6-1 124 0 0,-73 9 0 0 0,57 0 71 0 0,-190 36 3414 0 0,94-13-2775 0 0,144-29-1243 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1 1 1 0 0,-10 5-1 0 0,7-2-3387 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="46824.15">5265 2119 10680 0 0,'0'0'1129'0'0,"8"13"-2116"0"0,-6-10 867 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,1-1-1 0 0,0 7 0 0 0,4 38-564 0 0,-4-34 646 0 0,-1-6 39 0 0,4 62-29 0 0,-5-62 262 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-4 12 0 0 0,6-19-180 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-2-42 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1-2-1 0 0,-3-2-248 0 0,1 0-1 0 0,0-1 1 0 0,1 0-1 0 0,-6-9 0 0 0,3 0-84 0 0,0-2-1 0 0,0 0 0 0 0,2 0 0 0 0,0 0 1 0 0,-2-34-1 0 0,4 26-109 0 0,2-1 1 0 0,1 1-1 0 0,7-37 1 0 0,-5 50 1483 0 0,-4 19 0 0 0,-5 12-1056 0 0,-27 81-96 0 0,26-82 80 0 0,-1 0 0 0 0,0-1 0 0 0,-17 24 0 0 0,18-32 234 0 0,0-1 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0-2 1 0 0,0 0-1 0 0,-11 5 1 0 0,17-8 33 0 0,3-1-318 0 0,15 6 133 0 0,-8-6 64 0 0,0 0-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 0-1 0 0,10-2 1 0 0,-7 1-7 0 0,90-10-1363 0 0,-87 9 645 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="47630.7">6623 3050 11600 0 0,'0'0'2953'0'0,"-10"0"-2597"0"0,-98 5-353 0 0,75-2-15 0 0,-99 5 80 0 0,-106 24 756 0 0,209-27-776 0 0,-76 21 336 0 0,23-4-211 0 0,-17 2-83 0 0,-237 59-361 0 0,244-54-4225 0 0,84-27 1448 0 0,1-1-712 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="48602.97">5306 3202 9728 0 0,'0'0'744'0'0,"8"-16"-396"0"0,-7 13-50 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1-1 0 0,3-4 1 0 0,-4 4-18 0 0,-2 2-182 0 0,11 9-2 0 0,-9-4-74 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 8 0 0 0,1 17 81 0 0,0-30-101 0 0,3 21 118 0 0,-2 2 0 0 0,0-1 0 0 0,-4 35 1 0 0,-7-22 814 0 0,3-48-1107 0 0,4 5 3 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0-11 1 0 0,0 13 86 0 0,-3-112 43 0 0,4 107 79 0 0,0 1 1 0 0,1-1-1 0 0,0 2 1 0 0,4-17 0 0 0,2 11-790 0 0,-6 12-31 0 0,-9 10 374 0 0,3-2 404 0 0,0 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-6 10 0 0 0,-3 4 17 0 0,-13 15 205 0 0,-2-1 1 0 0,-36 31 0 0 0,63-63-198 0 0,-5 3 89 0 0,0 1 1 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-5 11 0 0 0,10-18-108 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 21 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,3 2 1 0 0,1-1 107 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,7 1 0 0 0,20-3-511 0 0,-1-1 0 0 0,0-2 1 0 0,46-12-1 0 0,-59 12-4731 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="52077.83">507 4723 9440 0 0,'0'0'721'0'0,"3"10"-569"0"0,0 42-1183 0 0,-1 21 285 0 0,-49 294 523 0 0,47-363 191 0 0,-2 7-163 0 0,0-1 1 0 0,-5 15-1 0 0,2-15-2574 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="52634.91">523 4751 9960 0 0,'0'0'994'0'0,"14"-9"-1236"0"0,32-10-1915 0 0,-11 7 104 0 0,26-14 2925 0 0,-36 17 103 0 0,-1 1-1 0 0,1 1 1 0 0,0 1-1 0 0,51-4 0 0 0,-9 1 36 0 0,-11 0-1035 0 0,71-13-142 0 0,-97 15 113 0 0,-1-1 1 0 0,33-14 0 0 0,35-14-121 0 0,-96 35 356 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="53419.87">468 5035 14368 0 0,'0'0'330'0'0,"-5"0"666"0"0,25-6-1308 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,36-2 1 0 0,-39 7 309 0 0,21 0 0 0 0,16 0-2 0 0,-51 0-33 0 0,52-7-1604 0 0,-45 5-2865 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="53823.04">1278 4619 9672 0 0,'0'0'1600'0'0,"-4"12"-974"0"0,-4 112-291 0 0,5-31-336 0 0,-2-40-55 0 0,-3 28-32 0 0,5 118 1 0 0,3-180-4226 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54243.75">1578 4964 11256 0 0,'0'0'2629'0'0,"1"6"-2172"0"0,-19 14-462 0 0,0 1-1 0 0,1 1 0 0 0,1-1 1 0 0,-18 37-1 0 0,31-52 192 0 0,1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-2 9 0 0 0,4-13-128 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,-1-2-44 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,1 0 0 0 0,-1 0-9 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,2-1 0 0 0,14-17 55 0 0,-7 8 16 0 0,-4 4-72 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,6-14-1 0 0,-11 21 147 0 0,2 2-65 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 2-1 0 0,8 18-337 0 0,23 54 1349 0 0,-26-64-2945 0 0,1-1-1 0 0,10 14 1 0 0,-12-19-3794 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54662.41">1917 4981 13304 0 0,'0'0'1333'0'0,"-4"2"-1246"0"0,-1 2-289 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-4 13 1 0 0,2-6 286 0 0,2 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,0 22 1 0 0,2-33 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,2 3 0 0 0,-3-3-55 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2 0-14 0 0,1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1-1 1 0 0,6-13-225 0 0,0 0-1 0 0,-1 0 1 0 0,6-27 0 0 0,6-18-173 0 0,-18 60 403 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,1-1 0 0 0,-1 2-9 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,3 6-4 0 0,1 0 0 0 0,-2 0 0 0 0,6 9-1 0 0,-9-15 8 0 0,11 27 2 0 0,-1 1 0 0 0,0-1-1 0 0,-2 1 1 0 0,6 34 0 0 0,-7-27 88 0 0,2 10 109 0 0,2 50 1 0 0,-4-35-100 0 0,3 102-178 0 0,-6-76-1039 0 0,-3-71 624 0 0,0-5-3 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="55265.65">3556 4531 11728 0 0,'0'0'688'0'0,"-2"-13"-376"0"0,4 15-335 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,2 4-1 0 0,7 32 40 0 0,-6-19 12 0 0,9 42 937 0 0,7 104 1 0 0,-11-77-344 0 0,-5-53-420 0 0,11 101-392 0 0,-12-50-3921 0 0,-4-70 2321 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="55917.21">3608 4458 17423 0 0,'0'0'844'0'0,"12"0"200"0"0,21 0-1352 0 0,57-8 0 0 0,-41 0 273 0 0,285-57-410 0 0,-40-8 285 0 0,-275 68 160 0 0,12-3 0 0 0,1 2 0 0 0,0 0 0 0 0,37 0 0 0 0,-65 6 8 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-2 1 0 0 0,2-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,5 3 1 0 0,-4 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,3 8-1 0 0,25 83-242 0 0,26 148-1 0 0,-32-130-287 0 0,-8-35-429 0 0,4-1 0 0 0,32 80-1 0 0,-46-144 958 0 0,0-1-1 0 0,1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,13 10-1 0 0,-21-21 12 0 0,0 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0-18 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0-1 1 0 0,-2-2-83 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 1 0 0,0-1-1 0 0,-9-4 0 0 0,-4 0-203 0 0,-1-1 0 0 0,0 0 0 0 0,-20-5 0 0 0,-5 1-121 0 0,-1 3 0 0 0,0 1 1 0 0,-50-3-1 0 0,28 6 987 0 0,-1 4 0 0 0,-1 2 0 0 0,-87 12 0 0 0,-197 49 5490 0 0,267-40-8371 0 0,65-15-711 0 0,-12 4-2806 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56954.85">3556 5875 14280 0 0,'0'0'1077'0'0,"2"-10"-586"0"0,-2 10-499 0 0,0 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,6 7-270 0 0,0 4 136 0 0,0 1 0 0 0,-1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-2 0 0 0 0,3 18 0 0 0,9 87-1752 0 0,-12-101 229 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57749.45">3529 5799 13560 0 0,'2'0'1485'0'0,"-1"0"-1484"0"0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,1 0 1 0 0,-1-1 6 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,1 2 0 0 0,13 2 195 0 0,51-17 557 0 0,88-13-361 0 0,159-38-239 0 0,-9-3 1366 0 0,-147 40-1100 0 0,-135 22-291 0 0,-19 4-121 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,5 2 0 0 0,-3-1-58 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 2 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,2 7 0 0 0,3 20-100 0 0,-2 0-1 0 0,-1 0 0 0 0,-2-1 1 0 0,-2 40-1 0 0,0-14 74 0 0,1-49 70 0 0,3 135 38 0 0,0-117 98 0 0,0 0-1 0 0,1 1 1 0 0,13 38-1 0 0,-13-53-133 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,9 11 0 0 0,-3-2 0 0 0,-10-18 1 0 0,-1-4-2 0 0,-4-4 15 0 0,-2 3 43 0 0,-1-1 0 0 0,0 1 1 0 0,0 1-1 0 0,-13-6 0 0 0,-7-4-10 0 0,17 9-36 0 0,0 0-1 0 0,-1 0 0 0 0,0 1 1 0 0,-12-2-1 0 0,0-1-9 0 0,-26-5-10 0 0,-93-9-1 0 0,-49 12 118 0 0,130 6 91 0 0,-10-1 456 0 0,-103 0 265 0 0,138 4-862 0 0,1 2 0 0 0,-67 13 1 0 0,-21 9 189 0 0,58-12-1585 0 0,1 2-4551 0 0,40-10 92 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="59228.66">3708 6101 10240 0 0,'0'0'593'0'0,"13"2"1527"0"0,-1 0-1065 0 0,-11-2-949 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,2-1 0 0 0,-2 0-37 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,5 2 0 0 0,-5-1-61 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,5-1 1 0 0,20-1-10 0 0,-24 2-13 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,3-2 0 0 0,-3 2 10 0 0,-3 0 4 0 0,1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1-4 0 0 0,-1 5 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-2-1 0 0 0,1-1 0 0 0,-1 0 2 0 0,1-1 1 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-7 0 0 0 0,-4 0 148 0 0,-9 2 67 0 0,20-1-179 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,-5-3-1 0 0,-7 0 216 0 0,2 5 145 0 0,5 0 64 0 0,8-2 264 0 0,0-8-610 0 0,1 7-121 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,18-15-163 0 0,-16 12 9 0 0,0 0-1 0 0,1 1 0 0 0,0 0 0 0 0,10-6 0 0 0,-9 6-692 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,10-8 0 0 0,-5 2-715 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="59659.6">3987 6019 13448 0 0,'0'0'298'0'0,"-8"7"745"0"0,3-1-677 0 0,5-6-369 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1-141 0 0,1 2 24 0 0,9 15 94 0 0,-5-11 30 0 0,-3-5-6 0 0,-1-2 24 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,8-7 704 0 0,-3 3-567 0 0,-6 4-148 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-2 1 0 0,12-20 349 0 0,-13 23-362 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,8 12-165 0 0,-7-12 134 0 0,1 5-272 0 0,0 1-1 0 0,0-1 1 0 0,6 10-1 0 0,-6-13-102 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="60044.21">4094 5846 6416 0 0,'0'0'184'0'0,"0"-1"-6"0"0,3-2-76 0 0,-3 2-57 0 0,0 1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,7 9 813 0 0,-2 13 50 0 0,-1 1 0 0 0,1 38 0 0 0,-6-42-385 0 0,2 1 0 0 0,0-1-1 0 0,8 39 1 0 0,-9-59-505 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,2-3-147 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,5-5 0 0 0,3-3-132 0 0,-9 9 224 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,0-2 0 0 0,5-10-52 0 0,-7 16 88 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,3 12 63 0 0,-3-7-88 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 3 0 0 0,-2 12-104 0 0,3-12-30 0 0,0 10-2066 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="60559.25">4236 6065 10680 0 0,'5'-11'810'0'0,"-4"9"-771"0"0,-1 1-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,3-1-1 0 0,0 0 272 0 0,-3 1-305 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 2 1 0 0,10 6-5 0 0,-1 2 0 0 0,-9-9 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,7 1-25 0 0,-9 0 56 0 0,0-1 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,2-1-16 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-6 0 0 0,3-9 13 0 0,-3 16 47 0 0,-1 0-344 0 0,1-5 1434 0 0,-1 5-1128 0 0,0 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,1 1-1 0 0,5 5-10 0 0,-5-5-47 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,1-1-257 0 0,-3 1 258 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 85 0 0,-1-3 65 0 0,1 0-44 0 0,-2 10-24 0 0,-2 4 24 0 0,-1 0 0 0 0,-6 13 0 0 0,0-4 116 0 0,-2 6-1138 0 0,13-25 935 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-6 23 0 0,0-4 16 0 0,0 8-53 0 0,0 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,1-3 1 0 0,-2 4-240 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="60925.75">4520 5965 8208 0 0,'0'0'393'0'0,"0"17"62"0"0,0-1 292 0 0,-1 1 0 0 0,-3 24 0 0 0,3-36-580 0 0,-1 7 743 0 0,7-20-799 0 0,9-10-641 0 0,-12 15 375 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,2-3 0 0 0,5-10-301 0 0,-9 15 454 0 0,0 1 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,6 1 141 0 0,-7-1-139 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,10 9-913 0 0,-4-6-2574 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="61268.52">4599 5695 15136 0 0,'0'0'17'0'0,"0"0"1"0"0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,9 8 492 0 0,7 14 53 0 0,-9-6-721 0 0,-1 0-1 0 0,-1-1 1 0 0,1 2-1 0 0,2 18 0 0 0,-4-17-57 0 0,40 197-4286 0 0,-40-188 206 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="61644.75">4454 5884 16208 0 0,'0'0'1233'0'0,"13"5"-683"0"0,129 29-788 0 0,-70-20-2046 0 0,-48-11-3337 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1145,10 +2481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D365BA88-6155-4091-8F9B-C33F8FA19836}">
-  <dimension ref="A15:E51"/>
+  <dimension ref="A15:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:E25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1157,9 +2493,13 @@
     <col min="2" max="2" width="13.9296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.06640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.9296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1173,8 +2513,14 @@
       <c r="E15" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
@@ -1188,8 +2534,20 @@
       <c r="E16" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
@@ -1203,8 +2561,20 @@
       <c r="E17" s="3">
         <v>148</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
@@ -1218,8 +2588,20 @@
       <c r="E18" s="3">
         <v>90</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P18" s="3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
@@ -1233,8 +2615,20 @@
       <c r="E19" s="4">
         <v>43831.03125</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P19" s="3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -1248,8 +2642,14 @@
       <c r="E20" s="4">
         <v>43831.043055555558</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="O20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P20" s="4">
+        <v>43831.020833333336</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
@@ -1259,8 +2659,14 @@
         <v>5</v>
       </c>
       <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="O21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P21" s="4">
+        <v>43831.072222222225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1270,15 +2676,19 @@
       <c r="E22" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="O22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
@@ -1293,7 +2703,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
@@ -1308,7 +2718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>3</v>
       </c>
@@ -1323,7 +2733,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
@@ -1338,7 +2748,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
@@ -1353,7 +2763,7 @@
         <v>43831.019444444442</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>15</v>
       </c>
@@ -1368,7 +2778,7 @@
         <v>43831.022916666669</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
@@ -1383,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>19</v>
       </c>
@@ -1398,7 +2808,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Updated Data Model document and Artifact 3 of write-up
</commit_message>
<xml_diff>
--- a/data/data_model.xlsx
+++ b/data/data_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7becb3257e745586/3_School/BootCamp_Springboard/Data_Engineering_Path/2_open_ended_capstone/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1225" documentId="8_{A2C35B67-1238-490E-AAF9-6F079BE219E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A080A3CE-17DD-462F-9AF0-460E2EB48195}"/>
+  <xr:revisionPtr revIDLastSave="1236" documentId="8_{A2C35B67-1238-490E-AAF9-6F079BE219E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A6D01E38-B5DD-413C-A8E5-742ECC76B7EC}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{6FAE3B8B-F522-441F-A816-43FE04CF5C89}"/>
+    <workbookView xWindow="6562" yWindow="3278" windowWidth="18225" windowHeight="11422" activeTab="1" xr2:uid="{6FAE3B8B-F522-441F-A816-43FE04CF5C89}"/>
   </bookViews>
   <sheets>
     <sheet name="bus_matrix" sheetId="7" r:id="rId1"/>
@@ -19,11 +19,11 @@
     <sheet name="physical_diagram" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1_data_catalog'!$A$1:$H$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1_data_catalog'!$A$1:$H$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="39" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="81">
   <si>
     <t>dispatching_base_num</t>
   </si>
@@ -261,30 +261,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>hour</t>
-  </si>
-  <si>
-    <t>date_id</t>
-  </si>
-  <si>
-    <t>num_day</t>
-  </si>
-  <si>
-    <t>day_description</t>
-  </si>
-  <si>
-    <t>month_description</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>week</t>
-  </si>
-  <si>
-    <t>week_description</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -292,6 +268,24 @@
   </si>
   <si>
     <t>Quick Rule of thumb!</t>
+  </si>
+  <si>
+    <t>day_of_week</t>
+  </si>
+  <si>
+    <t>day_number_in_epoch</t>
+  </si>
+  <si>
+    <t>week_number_in_epoch</t>
+  </si>
+  <si>
+    <t>month_number_in epoch</t>
+  </si>
+  <si>
+    <t>day_number_in_week</t>
+  </si>
+  <si>
+    <t>day_number_in_month</t>
   </si>
 </sst>
 </file>
@@ -588,12 +582,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,431 +602,17 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="126">
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
+  <dxfs count="42">
     <dxf>
       <font>
         <sz val="10"/>
@@ -2253,7 +1827,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4EBC4EC-550D-4AD2-B0DB-A8E6E702B3A5}" name="PivotTable2" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4EBC4EC-550D-4AD2-B0DB-A8E6E702B3A5}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C16:C24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -2387,13 +1961,13 @@
     <i/>
   </colItems>
   <formats count="28">
-    <format dxfId="111">
+    <format dxfId="27">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="110">
+    <format dxfId="26">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="109">
+    <format dxfId="25">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="3">
@@ -2404,10 +1978,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="108">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="107">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="3">
@@ -2421,7 +1995,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="106">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="2">
@@ -2434,7 +2008,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="105">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="2">
@@ -2447,7 +2021,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="104">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -2462,7 +2036,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="103">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -2477,7 +2051,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="102">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -2493,7 +2067,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="101">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -2510,7 +2084,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="100">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -2527,7 +2101,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="99">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -2543,7 +2117,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="98">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -2559,7 +2133,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="97">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2577,7 +2151,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2595,7 +2169,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="95">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2613,7 +2187,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="94">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2633,7 +2207,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2651,7 +2225,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2672,7 +2246,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2704,7 +2278,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2722,7 +2296,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2743,7 +2317,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2773,7 +2347,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2794,7 +2368,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2813,7 +2387,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2835,7 +2409,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -2868,7 +2442,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F22F06CB-A238-4D66-A7CC-240B62DA1572}" name="PivotTable1" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F22F06CB-A238-4D66-A7CC-240B62DA1572}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A16:A35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -3035,13 +2609,13 @@
     <i/>
   </colItems>
   <formats count="14">
-    <format dxfId="125">
+    <format dxfId="41">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="124">
+    <format dxfId="40">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="123">
+    <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="3">
@@ -3052,10 +2626,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="122">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="121">
+    <format dxfId="37">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="3">
@@ -3069,7 +2643,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="120">
+    <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="2">
@@ -3082,7 +2656,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="119">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="2">
@@ -3095,7 +2669,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="118">
+    <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3110,7 +2684,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="117">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3125,7 +2699,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="116">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3141,7 +2715,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="115">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3158,7 +2732,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="114">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3175,7 +2749,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="113">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3191,7 +2765,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="112">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3519,7 +3093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22065F7D-4203-49F7-AFCA-CAE5DDFF24A6}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J23" sqref="J23:L26"/>
     </sheetView>
   </sheetViews>
@@ -3531,13 +3105,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.4">
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:12" ht="70.900000000000006" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
@@ -3553,7 +3127,7 @@
         <v>50</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>16</v>
@@ -3572,181 +3146,181 @@
       <c r="A3" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:12" ht="14.25" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24" t="s">
-        <v>80</v>
+      <c r="B4" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27" t="s">
-        <v>80</v>
+      <c r="B5" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>80</v>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>80</v>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="19"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="19"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="16" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
     </row>
     <row r="17" spans="10:12" x14ac:dyDescent="0.4">
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
     </row>
     <row r="18" spans="10:12" x14ac:dyDescent="0.4">
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
     </row>
     <row r="19" spans="10:12" x14ac:dyDescent="0.4">
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="21" spans="10:12" x14ac:dyDescent="0.4">
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
     </row>
     <row r="22" spans="10:12" x14ac:dyDescent="0.4">
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
     </row>
     <row r="23" spans="10:12" x14ac:dyDescent="0.4">
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
     </row>
     <row r="24" spans="10:12" x14ac:dyDescent="0.4">
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
     </row>
     <row r="25" spans="10:12" x14ac:dyDescent="0.4">
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
     </row>
     <row r="26" spans="10:12" x14ac:dyDescent="0.4">
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3762,13 +3336,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2088174-295F-4FE5-8327-EA1891322AE8}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="F63" sqref="F63:H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5285,7 +4859,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B59" t="s">
         <v>5</v>
@@ -5394,7 +4968,7 @@
         <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>57</v>
@@ -5406,7 +4980,7 @@
         <v>69</v>
       </c>
       <c r="G64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H64" s="6" t="s">
         <v>57</v>
@@ -5417,10 +4991,10 @@
         <v>69</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
-      </c>
-      <c r="C65" t="s">
-        <v>47</v>
+        <v>75</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="E65" t="s">
         <v>63</v>
@@ -5429,10 +5003,10 @@
         <v>69</v>
       </c>
       <c r="G65" t="s">
-        <v>73</v>
-      </c>
-      <c r="H65" t="s">
-        <v>47</v>
+        <v>75</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.45">
@@ -5440,7 +5014,7 @@
         <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>57</v>
@@ -5452,7 +5026,7 @@
         <v>69</v>
       </c>
       <c r="G66" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H66" s="6" t="s">
         <v>57</v>
@@ -5463,7 +5037,7 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>57</v>
@@ -5475,7 +5049,7 @@
         <v>69</v>
       </c>
       <c r="G67" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H67" s="6" t="s">
         <v>57</v>
@@ -5486,7 +5060,7 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>57</v>
@@ -5498,7 +5072,7 @@
         <v>69</v>
       </c>
       <c r="G68" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>57</v>
@@ -5509,7 +5083,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>57</v>
@@ -5521,7 +5095,7 @@
         <v>69</v>
       </c>
       <c r="G69" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>57</v>
@@ -5532,7 +5106,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>57</v>
@@ -5544,60 +5118,14 @@
         <v>69</v>
       </c>
       <c r="G70" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H70" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
-        <v>69</v>
-      </c>
-      <c r="B71" t="s">
-        <v>78</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E71" t="s">
-        <v>63</v>
-      </c>
-      <c r="F71" t="s">
-        <v>69</v>
-      </c>
-      <c r="G71" t="s">
-        <v>78</v>
-      </c>
-      <c r="H71" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
-        <v>69</v>
-      </c>
-      <c r="B72" t="s">
-        <v>79</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E72" t="s">
-        <v>63</v>
-      </c>
-      <c r="F72" t="s">
-        <v>69</v>
-      </c>
-      <c r="G72" t="s">
-        <v>79</v>
-      </c>
-      <c r="H72" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:H72" xr:uid="{FFA2C0A9-B82F-4C34-8D2A-591A58EE8374}">
+  <autoFilter ref="A1:H70" xr:uid="{FFA2C0A9-B82F-4C34-8D2A-591A58EE8374}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H58">
       <sortCondition ref="A1"/>
     </sortState>
@@ -5611,7 +5139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCC4472-F4D9-449D-BCFE-57FF1B6C1123}">
   <dimension ref="A16:C103"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -5697,7 +5225,7 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C25"/>
     </row>
@@ -5753,208 +5281,208 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A47"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A48"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A49"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A50"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A51"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A52"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A53"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A54"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A55"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A56"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A57"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A58"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A59"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A60"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A61"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A62"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A63"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A64"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A65"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A66"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A67"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A68"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A69"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A70"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A71"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A72"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A73"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A74"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A75"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A76"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A77"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A78"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A79"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A80"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A81"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A82"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A83"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A84"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A85"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A86"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A87"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A88"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A89"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A90"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A91"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A92"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A93"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A94"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A95"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A96"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A97"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A98"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A99"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A100"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A101"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A102"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A103"/>
     </row>
   </sheetData>

</xml_diff>